<commit_message>
Simple converter version. (Direction only, Must require MIDI NoteNo )
</commit_message>
<xml_diff>
--- a/Template.xlsx
+++ b/Template.xlsx
@@ -8,7 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="Slot" sheetId="1" r:id="rId1"/>
-    <sheet name="Articulation" sheetId="2" r:id="rId2"/>
+    <sheet name="Articulation" sheetId="4" r:id="rId2"/>
     <sheet name="List(DO NOT MODIFY!)" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="139">
   <si>
     <t>Name</t>
     <phoneticPr fontId="1"/>
@@ -422,11 +422,26 @@
     <t>127:G8</t>
   </si>
   <si>
-    <t>NONE</t>
+    <t>Direction</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>NONE</t>
+    <t>Attribute</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Power Chord</t>
+  </si>
+  <si>
+    <t>Power Chord</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Name</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Power Code</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -434,7 +449,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -450,8 +465,17 @@
       <charset val="128"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="ＭＳ Ｐゴシック"/>
+      <family val="3"/>
+      <charset val="128"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -461,6 +485,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -494,7 +524,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -512,6 +542,18 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -826,7 +868,7 @@
     <col min="1" max="2" width="35.625" style="5" customWidth="1"/>
     <col min="3" max="3" width="10.5" style="4" customWidth="1"/>
     <col min="4" max="4" width="9.5" style="5" customWidth="1"/>
-    <col min="5" max="5" width="50.125" style="5" customWidth="1"/>
+    <col min="5" max="5" width="50.625" style="5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.15">
@@ -847,10 +889,14 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A2" s="3"/>
-      <c r="B2" s="3"/>
+      <c r="A2" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>135</v>
+      </c>
       <c r="C2" s="2" t="s">
-        <v>134</v>
+        <v>5</v>
       </c>
       <c r="D2" s="3">
         <v>120</v>
@@ -859,9 +905,9 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
+      <c r="B3" s="6"/>
       <c r="C3" s="2" t="s">
-        <v>134</v>
+        <v>5</v>
       </c>
       <c r="D3" s="3">
         <v>120</v>
@@ -870,9 +916,9 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A4" s="3"/>
-      <c r="B4" s="3"/>
+      <c r="B4" s="6"/>
       <c r="C4" s="2" t="s">
-        <v>134</v>
+        <v>5</v>
       </c>
       <c r="D4" s="3">
         <v>120</v>
@@ -881,9 +927,9 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
+      <c r="B5" s="6"/>
       <c r="C5" s="2" t="s">
-        <v>134</v>
+        <v>5</v>
       </c>
       <c r="D5" s="3">
         <v>120</v>
@@ -892,9 +938,9 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
+      <c r="B6" s="6"/>
       <c r="C6" s="2" t="s">
-        <v>134</v>
+        <v>5</v>
       </c>
       <c r="D6" s="3">
         <v>120</v>
@@ -903,9 +949,9 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
+      <c r="B7" s="6"/>
       <c r="C7" s="2" t="s">
-        <v>134</v>
+        <v>5</v>
       </c>
       <c r="D7" s="3">
         <v>120</v>
@@ -914,9 +960,9 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A8" s="3"/>
-      <c r="B8" s="3"/>
+      <c r="B8" s="6"/>
       <c r="C8" s="2" t="s">
-        <v>134</v>
+        <v>5</v>
       </c>
       <c r="D8" s="3">
         <v>120</v>
@@ -925,9 +971,9 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A9" s="3"/>
-      <c r="B9" s="3"/>
+      <c r="B9" s="6"/>
       <c r="C9" s="2" t="s">
-        <v>134</v>
+        <v>5</v>
       </c>
       <c r="D9" s="3">
         <v>120</v>
@@ -936,9 +982,9 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
+      <c r="B10" s="6"/>
       <c r="C10" s="2" t="s">
-        <v>134</v>
+        <v>5</v>
       </c>
       <c r="D10" s="3">
         <v>120</v>
@@ -947,9 +993,9 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A11" s="3"/>
-      <c r="B11" s="3"/>
+      <c r="B11" s="6"/>
       <c r="C11" s="2" t="s">
-        <v>134</v>
+        <v>5</v>
       </c>
       <c r="D11" s="3">
         <v>120</v>
@@ -958,9 +1004,9 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A12" s="3"/>
-      <c r="B12" s="3"/>
+      <c r="B12" s="6"/>
       <c r="C12" s="2" t="s">
-        <v>134</v>
+        <v>5</v>
       </c>
       <c r="D12" s="3">
         <v>120</v>
@@ -969,9 +1015,9 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A13" s="3"/>
-      <c r="B13" s="3"/>
+      <c r="B13" s="6"/>
       <c r="C13" s="2" t="s">
-        <v>134</v>
+        <v>5</v>
       </c>
       <c r="D13" s="3">
         <v>120</v>
@@ -980,9 +1026,9 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A14" s="3"/>
-      <c r="B14" s="3"/>
+      <c r="B14" s="6"/>
       <c r="C14" s="2" t="s">
-        <v>134</v>
+        <v>5</v>
       </c>
       <c r="D14" s="3">
         <v>120</v>
@@ -991,9 +1037,9 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A15" s="3"/>
-      <c r="B15" s="3"/>
+      <c r="B15" s="6"/>
       <c r="C15" s="2" t="s">
-        <v>134</v>
+        <v>5</v>
       </c>
       <c r="D15" s="3">
         <v>120</v>
@@ -1002,9 +1048,9 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A16" s="3"/>
-      <c r="B16" s="3"/>
+      <c r="B16" s="6"/>
       <c r="C16" s="2" t="s">
-        <v>134</v>
+        <v>5</v>
       </c>
       <c r="D16" s="3">
         <v>120</v>
@@ -1013,9 +1059,9 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A17" s="3"/>
-      <c r="B17" s="3"/>
+      <c r="B17" s="6"/>
       <c r="C17" s="2" t="s">
-        <v>134</v>
+        <v>5</v>
       </c>
       <c r="D17" s="3">
         <v>120</v>
@@ -1024,9 +1070,9 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A18" s="3"/>
-      <c r="B18" s="3"/>
+      <c r="B18" s="6"/>
       <c r="C18" s="2" t="s">
-        <v>134</v>
+        <v>5</v>
       </c>
       <c r="D18" s="3">
         <v>120</v>
@@ -1035,9 +1081,9 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A19" s="3"/>
-      <c r="B19" s="3"/>
+      <c r="B19" s="6"/>
       <c r="C19" s="2" t="s">
-        <v>134</v>
+        <v>5</v>
       </c>
       <c r="D19" s="3">
         <v>120</v>
@@ -1046,9 +1092,9 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A20" s="3"/>
-      <c r="B20" s="3"/>
+      <c r="B20" s="6"/>
       <c r="C20" s="2" t="s">
-        <v>134</v>
+        <v>5</v>
       </c>
       <c r="D20" s="3">
         <v>120</v>
@@ -1057,9 +1103,9 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A21" s="3"/>
-      <c r="B21" s="3"/>
+      <c r="B21" s="6"/>
       <c r="C21" s="2" t="s">
-        <v>134</v>
+        <v>5</v>
       </c>
       <c r="D21" s="3">
         <v>120</v>
@@ -1068,9 +1114,9 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A22" s="3"/>
-      <c r="B22" s="3"/>
+      <c r="B22" s="6"/>
       <c r="C22" s="2" t="s">
-        <v>134</v>
+        <v>5</v>
       </c>
       <c r="D22" s="3">
         <v>120</v>
@@ -1079,9 +1125,9 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A23" s="3"/>
-      <c r="B23" s="3"/>
+      <c r="B23" s="6"/>
       <c r="C23" s="2" t="s">
-        <v>134</v>
+        <v>5</v>
       </c>
       <c r="D23" s="3">
         <v>120</v>
@@ -1090,9 +1136,9 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A24" s="3"/>
-      <c r="B24" s="3"/>
+      <c r="B24" s="6"/>
       <c r="C24" s="2" t="s">
-        <v>134</v>
+        <v>5</v>
       </c>
       <c r="D24" s="3">
         <v>120</v>
@@ -1101,9 +1147,9 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A25" s="3"/>
-      <c r="B25" s="3"/>
+      <c r="B25" s="6"/>
       <c r="C25" s="2" t="s">
-        <v>134</v>
+        <v>5</v>
       </c>
       <c r="D25" s="3">
         <v>120</v>
@@ -1112,9 +1158,9 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A26" s="3"/>
-      <c r="B26" s="3"/>
+      <c r="B26" s="6"/>
       <c r="C26" s="2" t="s">
-        <v>134</v>
+        <v>5</v>
       </c>
       <c r="D26" s="3">
         <v>120</v>
@@ -1123,9 +1169,9 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A27" s="3"/>
-      <c r="B27" s="3"/>
+      <c r="B27" s="6"/>
       <c r="C27" s="2" t="s">
-        <v>134</v>
+        <v>5</v>
       </c>
       <c r="D27" s="3">
         <v>120</v>
@@ -1134,9 +1180,9 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A28" s="3"/>
-      <c r="B28" s="3"/>
+      <c r="B28" s="6"/>
       <c r="C28" s="2" t="s">
-        <v>134</v>
+        <v>5</v>
       </c>
       <c r="D28" s="3">
         <v>120</v>
@@ -1145,9 +1191,9 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A29" s="3"/>
-      <c r="B29" s="3"/>
+      <c r="B29" s="6"/>
       <c r="C29" s="2" t="s">
-        <v>134</v>
+        <v>5</v>
       </c>
       <c r="D29" s="3">
         <v>120</v>
@@ -1156,9 +1202,9 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A30" s="3"/>
-      <c r="B30" s="3"/>
+      <c r="B30" s="6"/>
       <c r="C30" s="2" t="s">
-        <v>134</v>
+        <v>5</v>
       </c>
       <c r="D30" s="3">
         <v>120</v>
@@ -1167,9 +1213,9 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A31" s="3"/>
-      <c r="B31" s="3"/>
+      <c r="B31" s="6"/>
       <c r="C31" s="2" t="s">
-        <v>134</v>
+        <v>5</v>
       </c>
       <c r="D31" s="3">
         <v>120</v>
@@ -1178,9 +1224,9 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A32" s="3"/>
-      <c r="B32" s="3"/>
+      <c r="B32" s="6"/>
       <c r="C32" s="2" t="s">
-        <v>134</v>
+        <v>5</v>
       </c>
       <c r="D32" s="3">
         <v>120</v>
@@ -1189,9 +1235,9 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A33" s="3"/>
-      <c r="B33" s="3"/>
+      <c r="B33" s="6"/>
       <c r="C33" s="2" t="s">
-        <v>134</v>
+        <v>5</v>
       </c>
       <c r="D33" s="3">
         <v>120</v>
@@ -1200,9 +1246,9 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A34" s="3"/>
-      <c r="B34" s="3"/>
+      <c r="B34" s="6"/>
       <c r="C34" s="2" t="s">
-        <v>134</v>
+        <v>5</v>
       </c>
       <c r="D34" s="3">
         <v>120</v>
@@ -1211,9 +1257,9 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A35" s="3"/>
-      <c r="B35" s="3"/>
+      <c r="B35" s="6"/>
       <c r="C35" s="2" t="s">
-        <v>134</v>
+        <v>5</v>
       </c>
       <c r="D35" s="3">
         <v>120</v>
@@ -1222,9 +1268,9 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A36" s="3"/>
-      <c r="B36" s="3"/>
+      <c r="B36" s="6"/>
       <c r="C36" s="2" t="s">
-        <v>134</v>
+        <v>5</v>
       </c>
       <c r="D36" s="3">
         <v>120</v>
@@ -1233,9 +1279,9 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A37" s="3"/>
-      <c r="B37" s="3"/>
+      <c r="B37" s="6"/>
       <c r="C37" s="2" t="s">
-        <v>134</v>
+        <v>5</v>
       </c>
       <c r="D37" s="3">
         <v>120</v>
@@ -1244,9 +1290,9 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A38" s="3"/>
-      <c r="B38" s="3"/>
+      <c r="B38" s="6"/>
       <c r="C38" s="2" t="s">
-        <v>134</v>
+        <v>5</v>
       </c>
       <c r="D38" s="3">
         <v>120</v>
@@ -1255,9 +1301,9 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A39" s="3"/>
-      <c r="B39" s="3"/>
+      <c r="B39" s="6"/>
       <c r="C39" s="2" t="s">
-        <v>134</v>
+        <v>5</v>
       </c>
       <c r="D39" s="3">
         <v>120</v>
@@ -1266,9 +1312,9 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A40" s="3"/>
-      <c r="B40" s="3"/>
+      <c r="B40" s="6"/>
       <c r="C40" s="2" t="s">
-        <v>134</v>
+        <v>5</v>
       </c>
       <c r="D40" s="3">
         <v>120</v>
@@ -1277,9 +1323,9 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A41" s="3"/>
-      <c r="B41" s="3"/>
+      <c r="B41" s="6"/>
       <c r="C41" s="2" t="s">
-        <v>134</v>
+        <v>5</v>
       </c>
       <c r="D41" s="3">
         <v>120</v>
@@ -1288,9 +1334,9 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A42" s="3"/>
-      <c r="B42" s="3"/>
+      <c r="B42" s="6"/>
       <c r="C42" s="2" t="s">
-        <v>134</v>
+        <v>5</v>
       </c>
       <c r="D42" s="3">
         <v>120</v>
@@ -1299,9 +1345,9 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A43" s="3"/>
-      <c r="B43" s="3"/>
+      <c r="B43" s="6"/>
       <c r="C43" s="2" t="s">
-        <v>134</v>
+        <v>5</v>
       </c>
       <c r="D43" s="3">
         <v>120</v>
@@ -1310,9 +1356,9 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A44" s="3"/>
-      <c r="B44" s="3"/>
+      <c r="B44" s="6"/>
       <c r="C44" s="2" t="s">
-        <v>134</v>
+        <v>5</v>
       </c>
       <c r="D44" s="3">
         <v>120</v>
@@ -1321,9 +1367,9 @@
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A45" s="3"/>
-      <c r="B45" s="3"/>
+      <c r="B45" s="6"/>
       <c r="C45" s="2" t="s">
-        <v>134</v>
+        <v>5</v>
       </c>
       <c r="D45" s="3">
         <v>120</v>
@@ -1332,9 +1378,9 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A46" s="3"/>
-      <c r="B46" s="3"/>
+      <c r="B46" s="6"/>
       <c r="C46" s="2" t="s">
-        <v>134</v>
+        <v>5</v>
       </c>
       <c r="D46" s="3">
         <v>120</v>
@@ -1343,9 +1389,9 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A47" s="3"/>
-      <c r="B47" s="3"/>
+      <c r="B47" s="6"/>
       <c r="C47" s="2" t="s">
-        <v>134</v>
+        <v>5</v>
       </c>
       <c r="D47" s="3">
         <v>120</v>
@@ -1354,9 +1400,9 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A48" s="3"/>
-      <c r="B48" s="3"/>
+      <c r="B48" s="6"/>
       <c r="C48" s="2" t="s">
-        <v>134</v>
+        <v>5</v>
       </c>
       <c r="D48" s="3">
         <v>120</v>
@@ -1365,9 +1411,9 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A49" s="3"/>
-      <c r="B49" s="3"/>
+      <c r="B49" s="6"/>
       <c r="C49" s="2" t="s">
-        <v>134</v>
+        <v>5</v>
       </c>
       <c r="D49" s="3">
         <v>120</v>
@@ -1376,9 +1422,9 @@
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A50" s="3"/>
-      <c r="B50" s="3"/>
+      <c r="B50" s="6"/>
       <c r="C50" s="2" t="s">
-        <v>134</v>
+        <v>5</v>
       </c>
       <c r="D50" s="3">
         <v>120</v>
@@ -1387,9 +1433,9 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A51" s="3"/>
-      <c r="B51" s="3"/>
+      <c r="B51" s="6"/>
       <c r="C51" s="2" t="s">
-        <v>134</v>
+        <v>5</v>
       </c>
       <c r="D51" s="3">
         <v>120</v>
@@ -1398,9 +1444,9 @@
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A52" s="3"/>
-      <c r="B52" s="3"/>
+      <c r="B52" s="6"/>
       <c r="C52" s="2" t="s">
-        <v>134</v>
+        <v>5</v>
       </c>
       <c r="D52" s="3">
         <v>120</v>
@@ -1409,9 +1455,9 @@
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A53" s="3"/>
-      <c r="B53" s="3"/>
+      <c r="B53" s="6"/>
       <c r="C53" s="2" t="s">
-        <v>134</v>
+        <v>5</v>
       </c>
       <c r="D53" s="3">
         <v>120</v>
@@ -1420,9 +1466,9 @@
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A54" s="3"/>
-      <c r="B54" s="3"/>
+      <c r="B54" s="6"/>
       <c r="C54" s="2" t="s">
-        <v>134</v>
+        <v>5</v>
       </c>
       <c r="D54" s="3">
         <v>120</v>
@@ -1431,9 +1477,9 @@
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A55" s="3"/>
-      <c r="B55" s="3"/>
+      <c r="B55" s="6"/>
       <c r="C55" s="2" t="s">
-        <v>134</v>
+        <v>5</v>
       </c>
       <c r="D55" s="3">
         <v>120</v>
@@ -1442,9 +1488,9 @@
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A56" s="3"/>
-      <c r="B56" s="3"/>
+      <c r="B56" s="6"/>
       <c r="C56" s="2" t="s">
-        <v>134</v>
+        <v>5</v>
       </c>
       <c r="D56" s="3">
         <v>120</v>
@@ -1453,9 +1499,9 @@
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A57" s="3"/>
-      <c r="B57" s="3"/>
+      <c r="B57" s="6"/>
       <c r="C57" s="2" t="s">
-        <v>134</v>
+        <v>5</v>
       </c>
       <c r="D57" s="3">
         <v>120</v>
@@ -1464,9 +1510,9 @@
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A58" s="3"/>
-      <c r="B58" s="3"/>
+      <c r="B58" s="6"/>
       <c r="C58" s="2" t="s">
-        <v>134</v>
+        <v>5</v>
       </c>
       <c r="D58" s="3">
         <v>120</v>
@@ -1475,9 +1521,9 @@
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A59" s="3"/>
-      <c r="B59" s="3"/>
+      <c r="B59" s="6"/>
       <c r="C59" s="2" t="s">
-        <v>134</v>
+        <v>5</v>
       </c>
       <c r="D59" s="3">
         <v>120</v>
@@ -1486,9 +1532,9 @@
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A60" s="3"/>
-      <c r="B60" s="3"/>
+      <c r="B60" s="6"/>
       <c r="C60" s="2" t="s">
-        <v>134</v>
+        <v>5</v>
       </c>
       <c r="D60" s="3">
         <v>120</v>
@@ -1497,9 +1543,9 @@
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A61" s="3"/>
-      <c r="B61" s="3"/>
+      <c r="B61" s="6"/>
       <c r="C61" s="2" t="s">
-        <v>134</v>
+        <v>5</v>
       </c>
       <c r="D61" s="3">
         <v>120</v>
@@ -1508,9 +1554,9 @@
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A62" s="3"/>
-      <c r="B62" s="3"/>
+      <c r="B62" s="6"/>
       <c r="C62" s="2" t="s">
-        <v>134</v>
+        <v>5</v>
       </c>
       <c r="D62" s="3">
         <v>120</v>
@@ -1519,9 +1565,9 @@
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A63" s="3"/>
-      <c r="B63" s="3"/>
+      <c r="B63" s="6"/>
       <c r="C63" s="2" t="s">
-        <v>134</v>
+        <v>5</v>
       </c>
       <c r="D63" s="3">
         <v>120</v>
@@ -1530,9 +1576,9 @@
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A64" s="3"/>
-      <c r="B64" s="3"/>
+      <c r="B64" s="6"/>
       <c r="C64" s="2" t="s">
-        <v>134</v>
+        <v>5</v>
       </c>
       <c r="D64" s="3">
         <v>120</v>
@@ -1541,9 +1587,9 @@
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A65" s="3"/>
-      <c r="B65" s="3"/>
+      <c r="B65" s="6"/>
       <c r="C65" s="2" t="s">
-        <v>134</v>
+        <v>5</v>
       </c>
       <c r="D65" s="3">
         <v>120</v>
@@ -1552,9 +1598,9 @@
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A66" s="3"/>
-      <c r="B66" s="3"/>
+      <c r="B66" s="6"/>
       <c r="C66" s="2" t="s">
-        <v>134</v>
+        <v>5</v>
       </c>
       <c r="D66" s="3">
         <v>120</v>
@@ -1563,9 +1609,9 @@
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A67" s="3"/>
-      <c r="B67" s="3"/>
+      <c r="B67" s="6"/>
       <c r="C67" s="2" t="s">
-        <v>134</v>
+        <v>5</v>
       </c>
       <c r="D67" s="3">
         <v>120</v>
@@ -1574,9 +1620,9 @@
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A68" s="3"/>
-      <c r="B68" s="3"/>
+      <c r="B68" s="6"/>
       <c r="C68" s="2" t="s">
-        <v>134</v>
+        <v>5</v>
       </c>
       <c r="D68" s="3">
         <v>120</v>
@@ -1585,9 +1631,9 @@
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A69" s="3"/>
-      <c r="B69" s="3"/>
+      <c r="B69" s="6"/>
       <c r="C69" s="2" t="s">
-        <v>134</v>
+        <v>5</v>
       </c>
       <c r="D69" s="3">
         <v>120</v>
@@ -1596,9 +1642,9 @@
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A70" s="3"/>
-      <c r="B70" s="3"/>
+      <c r="B70" s="6"/>
       <c r="C70" s="2" t="s">
-        <v>134</v>
+        <v>5</v>
       </c>
       <c r="D70" s="3">
         <v>120</v>
@@ -1607,9 +1653,9 @@
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A71" s="3"/>
-      <c r="B71" s="3"/>
+      <c r="B71" s="6"/>
       <c r="C71" s="2" t="s">
-        <v>134</v>
+        <v>5</v>
       </c>
       <c r="D71" s="3">
         <v>120</v>
@@ -1618,9 +1664,9 @@
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A72" s="3"/>
-      <c r="B72" s="3"/>
+      <c r="B72" s="6"/>
       <c r="C72" s="2" t="s">
-        <v>134</v>
+        <v>5</v>
       </c>
       <c r="D72" s="3">
         <v>120</v>
@@ -1629,9 +1675,9 @@
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A73" s="3"/>
-      <c r="B73" s="3"/>
+      <c r="B73" s="6"/>
       <c r="C73" s="2" t="s">
-        <v>134</v>
+        <v>5</v>
       </c>
       <c r="D73" s="3">
         <v>120</v>
@@ -1640,9 +1686,9 @@
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A74" s="3"/>
-      <c r="B74" s="3"/>
+      <c r="B74" s="6"/>
       <c r="C74" s="2" t="s">
-        <v>134</v>
+        <v>5</v>
       </c>
       <c r="D74" s="3">
         <v>120</v>
@@ -1651,9 +1697,9 @@
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A75" s="3"/>
-      <c r="B75" s="3"/>
+      <c r="B75" s="6"/>
       <c r="C75" s="2" t="s">
-        <v>134</v>
+        <v>5</v>
       </c>
       <c r="D75" s="3">
         <v>120</v>
@@ -1662,9 +1708,9 @@
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A76" s="3"/>
-      <c r="B76" s="3"/>
+      <c r="B76" s="6"/>
       <c r="C76" s="2" t="s">
-        <v>134</v>
+        <v>5</v>
       </c>
       <c r="D76" s="3">
         <v>120</v>
@@ -1673,9 +1719,9 @@
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A77" s="3"/>
-      <c r="B77" s="3"/>
+      <c r="B77" s="6"/>
       <c r="C77" s="2" t="s">
-        <v>134</v>
+        <v>5</v>
       </c>
       <c r="D77" s="3">
         <v>120</v>
@@ -1684,9 +1730,9 @@
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A78" s="3"/>
-      <c r="B78" s="3"/>
+      <c r="B78" s="6"/>
       <c r="C78" s="2" t="s">
-        <v>134</v>
+        <v>5</v>
       </c>
       <c r="D78" s="3">
         <v>120</v>
@@ -1695,9 +1741,9 @@
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A79" s="3"/>
-      <c r="B79" s="3"/>
+      <c r="B79" s="6"/>
       <c r="C79" s="2" t="s">
-        <v>134</v>
+        <v>5</v>
       </c>
       <c r="D79" s="3">
         <v>120</v>
@@ -1706,9 +1752,9 @@
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A80" s="3"/>
-      <c r="B80" s="3"/>
+      <c r="B80" s="6"/>
       <c r="C80" s="2" t="s">
-        <v>134</v>
+        <v>5</v>
       </c>
       <c r="D80" s="3">
         <v>120</v>
@@ -1717,9 +1763,9 @@
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A81" s="3"/>
-      <c r="B81" s="3"/>
+      <c r="B81" s="6"/>
       <c r="C81" s="2" t="s">
-        <v>134</v>
+        <v>5</v>
       </c>
       <c r="D81" s="3">
         <v>120</v>
@@ -1728,9 +1774,9 @@
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A82" s="3"/>
-      <c r="B82" s="3"/>
+      <c r="B82" s="6"/>
       <c r="C82" s="2" t="s">
-        <v>134</v>
+        <v>5</v>
       </c>
       <c r="D82" s="3">
         <v>120</v>
@@ -1739,9 +1785,9 @@
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A83" s="3"/>
-      <c r="B83" s="3"/>
+      <c r="B83" s="6"/>
       <c r="C83" s="2" t="s">
-        <v>134</v>
+        <v>5</v>
       </c>
       <c r="D83" s="3">
         <v>120</v>
@@ -1750,9 +1796,9 @@
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A84" s="3"/>
-      <c r="B84" s="3"/>
+      <c r="B84" s="6"/>
       <c r="C84" s="2" t="s">
-        <v>134</v>
+        <v>5</v>
       </c>
       <c r="D84" s="3">
         <v>120</v>
@@ -1761,9 +1807,9 @@
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A85" s="3"/>
-      <c r="B85" s="3"/>
+      <c r="B85" s="6"/>
       <c r="C85" s="2" t="s">
-        <v>134</v>
+        <v>5</v>
       </c>
       <c r="D85" s="3">
         <v>120</v>
@@ -1772,9 +1818,9 @@
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A86" s="3"/>
-      <c r="B86" s="3"/>
+      <c r="B86" s="6"/>
       <c r="C86" s="2" t="s">
-        <v>134</v>
+        <v>5</v>
       </c>
       <c r="D86" s="3">
         <v>120</v>
@@ -1783,9 +1829,9 @@
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A87" s="3"/>
-      <c r="B87" s="3"/>
+      <c r="B87" s="6"/>
       <c r="C87" s="2" t="s">
-        <v>134</v>
+        <v>5</v>
       </c>
       <c r="D87" s="3">
         <v>120</v>
@@ -1794,9 +1840,9 @@
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A88" s="3"/>
-      <c r="B88" s="3"/>
+      <c r="B88" s="6"/>
       <c r="C88" s="2" t="s">
-        <v>134</v>
+        <v>5</v>
       </c>
       <c r="D88" s="3">
         <v>120</v>
@@ -1805,9 +1851,9 @@
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A89" s="3"/>
-      <c r="B89" s="3"/>
+      <c r="B89" s="6"/>
       <c r="C89" s="2" t="s">
-        <v>134</v>
+        <v>5</v>
       </c>
       <c r="D89" s="3">
         <v>120</v>
@@ -1816,9 +1862,9 @@
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A90" s="3"/>
-      <c r="B90" s="3"/>
+      <c r="B90" s="6"/>
       <c r="C90" s="2" t="s">
-        <v>134</v>
+        <v>5</v>
       </c>
       <c r="D90" s="3">
         <v>120</v>
@@ -1827,9 +1873,9 @@
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A91" s="3"/>
-      <c r="B91" s="3"/>
+      <c r="B91" s="6"/>
       <c r="C91" s="2" t="s">
-        <v>134</v>
+        <v>5</v>
       </c>
       <c r="D91" s="3">
         <v>120</v>
@@ -1838,9 +1884,9 @@
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A92" s="3"/>
-      <c r="B92" s="3"/>
+      <c r="B92" s="6"/>
       <c r="C92" s="2" t="s">
-        <v>134</v>
+        <v>5</v>
       </c>
       <c r="D92" s="3">
         <v>120</v>
@@ -1849,9 +1895,9 @@
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A93" s="3"/>
-      <c r="B93" s="3"/>
+      <c r="B93" s="6"/>
       <c r="C93" s="2" t="s">
-        <v>134</v>
+        <v>5</v>
       </c>
       <c r="D93" s="3">
         <v>120</v>
@@ -1860,9 +1906,9 @@
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A94" s="3"/>
-      <c r="B94" s="3"/>
+      <c r="B94" s="6"/>
       <c r="C94" s="2" t="s">
-        <v>134</v>
+        <v>5</v>
       </c>
       <c r="D94" s="3">
         <v>120</v>
@@ -1871,9 +1917,9 @@
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A95" s="3"/>
-      <c r="B95" s="3"/>
+      <c r="B95" s="6"/>
       <c r="C95" s="2" t="s">
-        <v>134</v>
+        <v>5</v>
       </c>
       <c r="D95" s="3">
         <v>120</v>
@@ -1882,9 +1928,9 @@
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A96" s="3"/>
-      <c r="B96" s="3"/>
+      <c r="B96" s="6"/>
       <c r="C96" s="2" t="s">
-        <v>134</v>
+        <v>5</v>
       </c>
       <c r="D96" s="3">
         <v>120</v>
@@ -1893,9 +1939,9 @@
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A97" s="3"/>
-      <c r="B97" s="3"/>
+      <c r="B97" s="6"/>
       <c r="C97" s="2" t="s">
-        <v>134</v>
+        <v>5</v>
       </c>
       <c r="D97" s="3">
         <v>120</v>
@@ -1904,9 +1950,9 @@
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A98" s="3"/>
-      <c r="B98" s="3"/>
+      <c r="B98" s="6"/>
       <c r="C98" s="2" t="s">
-        <v>134</v>
+        <v>5</v>
       </c>
       <c r="D98" s="3">
         <v>120</v>
@@ -1915,9 +1961,9 @@
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A99" s="3"/>
-      <c r="B99" s="3"/>
+      <c r="B99" s="6"/>
       <c r="C99" s="2" t="s">
-        <v>134</v>
+        <v>5</v>
       </c>
       <c r="D99" s="3">
         <v>120</v>
@@ -1926,9 +1972,9 @@
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A100" s="3"/>
-      <c r="B100" s="3"/>
+      <c r="B100" s="6"/>
       <c r="C100" s="2" t="s">
-        <v>134</v>
+        <v>5</v>
       </c>
       <c r="D100" s="3">
         <v>120</v>
@@ -1937,9 +1983,9 @@
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A101" s="3"/>
-      <c r="B101" s="3"/>
+      <c r="B101" s="6"/>
       <c r="C101" s="2" t="s">
-        <v>134</v>
+        <v>5</v>
       </c>
       <c r="D101" s="3">
         <v>120</v>
@@ -1948,9 +1994,9 @@
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A102" s="3"/>
-      <c r="B102" s="3"/>
+      <c r="B102" s="6"/>
       <c r="C102" s="2" t="s">
-        <v>134</v>
+        <v>5</v>
       </c>
       <c r="D102" s="3">
         <v>120</v>
@@ -1959,9 +2005,9 @@
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A103" s="3"/>
-      <c r="B103" s="3"/>
+      <c r="B103" s="6"/>
       <c r="C103" s="2" t="s">
-        <v>134</v>
+        <v>5</v>
       </c>
       <c r="D103" s="3">
         <v>120</v>
@@ -1970,9 +2016,9 @@
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A104" s="3"/>
-      <c r="B104" s="3"/>
+      <c r="B104" s="6"/>
       <c r="C104" s="2" t="s">
-        <v>134</v>
+        <v>5</v>
       </c>
       <c r="D104" s="3">
         <v>120</v>
@@ -1981,9 +2027,9 @@
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A105" s="3"/>
-      <c r="B105" s="3"/>
+      <c r="B105" s="6"/>
       <c r="C105" s="2" t="s">
-        <v>134</v>
+        <v>5</v>
       </c>
       <c r="D105" s="3">
         <v>120</v>
@@ -1992,9 +2038,9 @@
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A106" s="3"/>
-      <c r="B106" s="3"/>
+      <c r="B106" s="6"/>
       <c r="C106" s="2" t="s">
-        <v>134</v>
+        <v>5</v>
       </c>
       <c r="D106" s="3">
         <v>120</v>
@@ -2003,9 +2049,9 @@
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A107" s="3"/>
-      <c r="B107" s="3"/>
+      <c r="B107" s="6"/>
       <c r="C107" s="2" t="s">
-        <v>134</v>
+        <v>5</v>
       </c>
       <c r="D107" s="3">
         <v>120</v>
@@ -2014,9 +2060,9 @@
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A108" s="3"/>
-      <c r="B108" s="3"/>
+      <c r="B108" s="6"/>
       <c r="C108" s="2" t="s">
-        <v>134</v>
+        <v>5</v>
       </c>
       <c r="D108" s="3">
         <v>120</v>
@@ -2025,9 +2071,9 @@
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A109" s="3"/>
-      <c r="B109" s="3"/>
+      <c r="B109" s="6"/>
       <c r="C109" s="2" t="s">
-        <v>134</v>
+        <v>5</v>
       </c>
       <c r="D109" s="3">
         <v>120</v>
@@ -2036,9 +2082,9 @@
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A110" s="3"/>
-      <c r="B110" s="3"/>
+      <c r="B110" s="6"/>
       <c r="C110" s="2" t="s">
-        <v>134</v>
+        <v>5</v>
       </c>
       <c r="D110" s="3">
         <v>120</v>
@@ -2047,9 +2093,9 @@
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A111" s="3"/>
-      <c r="B111" s="3"/>
+      <c r="B111" s="6"/>
       <c r="C111" s="2" t="s">
-        <v>134</v>
+        <v>5</v>
       </c>
       <c r="D111" s="3">
         <v>120</v>
@@ -2058,9 +2104,9 @@
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A112" s="3"/>
-      <c r="B112" s="3"/>
+      <c r="B112" s="6"/>
       <c r="C112" s="2" t="s">
-        <v>134</v>
+        <v>5</v>
       </c>
       <c r="D112" s="3">
         <v>120</v>
@@ -2069,9 +2115,9 @@
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A113" s="3"/>
-      <c r="B113" s="3"/>
+      <c r="B113" s="6"/>
       <c r="C113" s="2" t="s">
-        <v>134</v>
+        <v>5</v>
       </c>
       <c r="D113" s="3">
         <v>120</v>
@@ -2080,9 +2126,9 @@
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A114" s="3"/>
-      <c r="B114" s="3"/>
+      <c r="B114" s="6"/>
       <c r="C114" s="2" t="s">
-        <v>134</v>
+        <v>5</v>
       </c>
       <c r="D114" s="3">
         <v>120</v>
@@ -2091,9 +2137,9 @@
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A115" s="3"/>
-      <c r="B115" s="3"/>
+      <c r="B115" s="6"/>
       <c r="C115" s="2" t="s">
-        <v>134</v>
+        <v>5</v>
       </c>
       <c r="D115" s="3">
         <v>120</v>
@@ -2102,9 +2148,9 @@
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A116" s="3"/>
-      <c r="B116" s="3"/>
+      <c r="B116" s="6"/>
       <c r="C116" s="2" t="s">
-        <v>134</v>
+        <v>5</v>
       </c>
       <c r="D116" s="3">
         <v>120</v>
@@ -2113,9 +2159,9 @@
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A117" s="3"/>
-      <c r="B117" s="3"/>
+      <c r="B117" s="6"/>
       <c r="C117" s="2" t="s">
-        <v>134</v>
+        <v>5</v>
       </c>
       <c r="D117" s="3">
         <v>120</v>
@@ -2124,9 +2170,9 @@
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A118" s="3"/>
-      <c r="B118" s="3"/>
+      <c r="B118" s="6"/>
       <c r="C118" s="2" t="s">
-        <v>134</v>
+        <v>5</v>
       </c>
       <c r="D118" s="3">
         <v>120</v>
@@ -2135,9 +2181,9 @@
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A119" s="3"/>
-      <c r="B119" s="3"/>
+      <c r="B119" s="6"/>
       <c r="C119" s="2" t="s">
-        <v>134</v>
+        <v>5</v>
       </c>
       <c r="D119" s="3">
         <v>120</v>
@@ -2146,9 +2192,9 @@
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A120" s="3"/>
-      <c r="B120" s="3"/>
+      <c r="B120" s="6"/>
       <c r="C120" s="2" t="s">
-        <v>134</v>
+        <v>5</v>
       </c>
       <c r="D120" s="3">
         <v>120</v>
@@ -2157,9 +2203,9 @@
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A121" s="3"/>
-      <c r="B121" s="3"/>
+      <c r="B121" s="6"/>
       <c r="C121" s="2" t="s">
-        <v>134</v>
+        <v>5</v>
       </c>
       <c r="D121" s="3">
         <v>120</v>
@@ -2168,9 +2214,9 @@
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A122" s="3"/>
-      <c r="B122" s="3"/>
+      <c r="B122" s="6"/>
       <c r="C122" s="2" t="s">
-        <v>134</v>
+        <v>5</v>
       </c>
       <c r="D122" s="3">
         <v>120</v>
@@ -2179,9 +2225,9 @@
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A123" s="3"/>
-      <c r="B123" s="3"/>
+      <c r="B123" s="6"/>
       <c r="C123" s="2" t="s">
-        <v>134</v>
+        <v>5</v>
       </c>
       <c r="D123" s="3">
         <v>120</v>
@@ -2190,9 +2236,9 @@
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A124" s="3"/>
-      <c r="B124" s="3"/>
+      <c r="B124" s="6"/>
       <c r="C124" s="2" t="s">
-        <v>134</v>
+        <v>5</v>
       </c>
       <c r="D124" s="3">
         <v>120</v>
@@ -2201,9 +2247,9 @@
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A125" s="3"/>
-      <c r="B125" s="3"/>
+      <c r="B125" s="6"/>
       <c r="C125" s="2" t="s">
-        <v>134</v>
+        <v>5</v>
       </c>
       <c r="D125" s="3">
         <v>120</v>
@@ -2212,9 +2258,9 @@
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A126" s="3"/>
-      <c r="B126" s="3"/>
+      <c r="B126" s="6"/>
       <c r="C126" s="2" t="s">
-        <v>134</v>
+        <v>5</v>
       </c>
       <c r="D126" s="3">
         <v>120</v>
@@ -2223,9 +2269,9 @@
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A127" s="3"/>
-      <c r="B127" s="3"/>
+      <c r="B127" s="6"/>
       <c r="C127" s="2" t="s">
-        <v>134</v>
+        <v>5</v>
       </c>
       <c r="D127" s="3">
         <v>120</v>
@@ -2234,9 +2280,9 @@
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A128" s="3"/>
-      <c r="B128" s="3"/>
+      <c r="B128" s="6"/>
       <c r="C128" s="2" t="s">
-        <v>134</v>
+        <v>5</v>
       </c>
       <c r="D128" s="3">
         <v>120</v>
@@ -2245,9 +2291,9 @@
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A129" s="3"/>
-      <c r="B129" s="3"/>
+      <c r="B129" s="6"/>
       <c r="C129" s="2" t="s">
-        <v>134</v>
+        <v>5</v>
       </c>
       <c r="D129" s="3">
         <v>120</v>
@@ -2260,10 +2306,16 @@
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
         <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>'List(DO NOT MODIFY!)'!$A$1:$A$129</xm:f>
+            <xm:f>Articulation!$A$2:$A$129</xm:f>
+          </x14:formula1>
+          <xm:sqref>B2:B129</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>'List(DO NOT MODIFY!)'!$A$1:$A$128</xm:f>
           </x14:formula1>
           <xm:sqref>C2:C129</xm:sqref>
         </x14:dataValidation>
@@ -2275,14 +2327,542 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B129"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="35.625" style="8" customWidth="1"/>
+    <col min="2" max="2" width="50.625" style="8" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A1" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A2" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="B2" s="7"/>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3" s="7"/>
+      <c r="B3" s="7"/>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A4" s="7"/>
+      <c r="B4" s="7"/>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A5" s="7"/>
+      <c r="B5" s="7"/>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A6" s="7"/>
+      <c r="B6" s="7"/>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A7" s="7"/>
+      <c r="B7" s="7"/>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A8" s="7"/>
+      <c r="B8" s="7"/>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A9" s="7"/>
+      <c r="B9" s="7"/>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A10" s="7"/>
+      <c r="B10" s="7"/>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A11" s="7"/>
+      <c r="B11" s="7"/>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A12" s="7"/>
+      <c r="B12" s="7"/>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A13" s="7"/>
+      <c r="B13" s="7"/>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A14" s="7"/>
+      <c r="B14" s="7"/>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A15" s="7"/>
+      <c r="B15" s="7"/>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A16" s="7"/>
+      <c r="B16" s="7"/>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A17" s="7"/>
+      <c r="B17" s="7"/>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A18" s="7"/>
+      <c r="B18" s="7"/>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A19" s="7"/>
+      <c r="B19" s="7"/>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A20" s="7"/>
+      <c r="B20" s="7"/>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A21" s="7"/>
+      <c r="B21" s="7"/>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A22" s="7"/>
+      <c r="B22" s="7"/>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A23" s="7"/>
+      <c r="B23" s="7"/>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A24" s="7"/>
+      <c r="B24" s="7"/>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A25" s="7"/>
+      <c r="B25" s="7"/>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A26" s="7"/>
+      <c r="B26" s="7"/>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A27" s="7"/>
+      <c r="B27" s="7"/>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A28" s="7"/>
+      <c r="B28" s="7"/>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A29" s="7"/>
+      <c r="B29" s="7"/>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A30" s="7"/>
+      <c r="B30" s="7"/>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A31" s="7"/>
+      <c r="B31" s="7"/>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A32" s="7"/>
+      <c r="B32" s="7"/>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A33" s="7"/>
+      <c r="B33" s="7"/>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A34" s="7"/>
+      <c r="B34" s="7"/>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A35" s="7"/>
+      <c r="B35" s="7"/>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A36" s="7"/>
+      <c r="B36" s="7"/>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A37" s="7"/>
+      <c r="B37" s="7"/>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A38" s="7"/>
+      <c r="B38" s="7"/>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A39" s="7"/>
+      <c r="B39" s="7"/>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A40" s="7"/>
+      <c r="B40" s="7"/>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A41" s="7"/>
+      <c r="B41" s="7"/>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A42" s="7"/>
+      <c r="B42" s="7"/>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A43" s="7"/>
+      <c r="B43" s="7"/>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A44" s="7"/>
+      <c r="B44" s="7"/>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A45" s="7"/>
+      <c r="B45" s="7"/>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A46" s="7"/>
+      <c r="B46" s="7"/>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A47" s="7"/>
+      <c r="B47" s="7"/>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A48" s="7"/>
+      <c r="B48" s="7"/>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A49" s="7"/>
+      <c r="B49" s="7"/>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A50" s="7"/>
+      <c r="B50" s="7"/>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A51" s="7"/>
+      <c r="B51" s="7"/>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A52" s="7"/>
+      <c r="B52" s="7"/>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A53" s="7"/>
+      <c r="B53" s="7"/>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A54" s="7"/>
+      <c r="B54" s="7"/>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A55" s="7"/>
+      <c r="B55" s="7"/>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A56" s="7"/>
+      <c r="B56" s="7"/>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A57" s="7"/>
+      <c r="B57" s="7"/>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A58" s="7"/>
+      <c r="B58" s="7"/>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A59" s="7"/>
+      <c r="B59" s="7"/>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A60" s="7"/>
+      <c r="B60" s="7"/>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A61" s="7"/>
+      <c r="B61" s="7"/>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A62" s="7"/>
+      <c r="B62" s="7"/>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A63" s="7"/>
+      <c r="B63" s="7"/>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A64" s="7"/>
+      <c r="B64" s="7"/>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A65" s="7"/>
+      <c r="B65" s="7"/>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A66" s="7"/>
+      <c r="B66" s="7"/>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A67" s="7"/>
+      <c r="B67" s="7"/>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A68" s="7"/>
+      <c r="B68" s="7"/>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A69" s="7"/>
+      <c r="B69" s="7"/>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A70" s="7"/>
+      <c r="B70" s="7"/>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A71" s="7"/>
+      <c r="B71" s="7"/>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A72" s="7"/>
+      <c r="B72" s="7"/>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A73" s="7"/>
+      <c r="B73" s="7"/>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A74" s="7"/>
+      <c r="B74" s="7"/>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A75" s="7"/>
+      <c r="B75" s="7"/>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A76" s="7"/>
+      <c r="B76" s="7"/>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A77" s="7"/>
+      <c r="B77" s="7"/>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A78" s="7"/>
+      <c r="B78" s="7"/>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A79" s="7"/>
+      <c r="B79" s="7"/>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A80" s="7"/>
+      <c r="B80" s="7"/>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A81" s="7"/>
+      <c r="B81" s="7"/>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A82" s="7"/>
+      <c r="B82" s="7"/>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A83" s="7"/>
+      <c r="B83" s="7"/>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A84" s="7"/>
+      <c r="B84" s="7"/>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A85" s="7"/>
+      <c r="B85" s="7"/>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A86" s="7"/>
+      <c r="B86" s="7"/>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A87" s="7"/>
+      <c r="B87" s="7"/>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A88" s="7"/>
+      <c r="B88" s="7"/>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A89" s="7"/>
+      <c r="B89" s="7"/>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A90" s="7"/>
+      <c r="B90" s="7"/>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A91" s="7"/>
+      <c r="B91" s="7"/>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A92" s="7"/>
+      <c r="B92" s="7"/>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A93" s="7"/>
+      <c r="B93" s="7"/>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A94" s="7"/>
+      <c r="B94" s="7"/>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A95" s="7"/>
+      <c r="B95" s="7"/>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A96" s="7"/>
+      <c r="B96" s="7"/>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A97" s="7"/>
+      <c r="B97" s="7"/>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A98" s="7"/>
+      <c r="B98" s="7"/>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A99" s="7"/>
+      <c r="B99" s="7"/>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A100" s="7"/>
+      <c r="B100" s="7"/>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A101" s="7"/>
+      <c r="B101" s="7"/>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A102" s="7"/>
+      <c r="B102" s="7"/>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A103" s="7"/>
+      <c r="B103" s="7"/>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A104" s="7"/>
+      <c r="B104" s="7"/>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A105" s="7"/>
+      <c r="B105" s="7"/>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A106" s="7"/>
+      <c r="B106" s="7"/>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A107" s="7"/>
+      <c r="B107" s="7"/>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A108" s="7"/>
+      <c r="B108" s="7"/>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A109" s="7"/>
+      <c r="B109" s="7"/>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A110" s="7"/>
+      <c r="B110" s="7"/>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A111" s="7"/>
+      <c r="B111" s="7"/>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A112" s="7"/>
+      <c r="B112" s="7"/>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A113" s="7"/>
+      <c r="B113" s="7"/>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A114" s="7"/>
+      <c r="B114" s="7"/>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A115" s="7"/>
+      <c r="B115" s="7"/>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A116" s="7"/>
+      <c r="B116" s="7"/>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A117" s="7"/>
+      <c r="B117" s="7"/>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A118" s="7"/>
+      <c r="B118" s="7"/>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A119" s="7"/>
+      <c r="B119" s="7"/>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A120" s="7"/>
+      <c r="B120" s="7"/>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A121" s="7"/>
+      <c r="B121" s="7"/>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A122" s="7"/>
+      <c r="B122" s="7"/>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A123" s="7"/>
+      <c r="B123" s="7"/>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A124" s="7"/>
+      <c r="B124" s="7"/>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A125" s="7"/>
+      <c r="B125" s="7"/>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A126" s="7"/>
+      <c r="B126" s="7"/>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A127" s="7"/>
+      <c r="B127" s="7"/>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A128" s="7"/>
+      <c r="B128" s="7"/>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A129" s="7"/>
+      <c r="B129" s="7"/>
+    </row>
+  </sheetData>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2291,662 +2871,664 @@
   <sheetPr>
     <tabColor theme="1"/>
   </sheetPr>
-  <dimension ref="A1:A129"/>
+  <dimension ref="A1:B128"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A109" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="9.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.15">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.15">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.15">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.15">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.15">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.15">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.15">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.15">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.15">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.15">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.15">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.15">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.15">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A22" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A23" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A24" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A25" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A26" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A27" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A28" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A29" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A30" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A31" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A32" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A33" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A34" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A35" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A36" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A37" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A38" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A39" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A40" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A41" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A42" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A43" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A44" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A45" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A46" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A47" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A48" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A49" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A50" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A51" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A52" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A53" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A54" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A55" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A56" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A57" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A58" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A59" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A60" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A61" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A62" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A63" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A64" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A65" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A66" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A67" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A68" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A69" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A70" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A71" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A72" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A73" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A74" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A75" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A76" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A77" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A78" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A79" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A80" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A81" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A82" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A83" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A84" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A85" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A86" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A87" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A88" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A89" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A90" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A91" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A92" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A93" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A94" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A95" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A96" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A97" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A98" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A99" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A100" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A101" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A102" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A103" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A104" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A105" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A106" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A107" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A108" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A109" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A110" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A111" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="112" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A112" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A113" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A114" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A115" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A116" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A117" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A118" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="119" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A119" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
     <row r="120" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A120" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A121" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row r="122" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A122" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
     <row r="123" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A123" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="124" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A124" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="125" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A125" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="126" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A126" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="127" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A127" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="128" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A128" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="129" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A129" t="s">
         <v>132</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Version 0.7: Spreadsheet format changed (compatible with v0.6.x)
</commit_message>
<xml_diff>
--- a/Template.xlsx
+++ b/Template.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
     <workbookView xWindow="2385" yWindow="3945" windowWidth="24825" windowHeight="15615" tabRatio="500"/>
@@ -11,14 +11,6 @@
     <sheet name="DO NOT MODIFY!" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0" iterateDelta="1E-4" concurrentCalc="0"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
-    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
-      <loext:extCalcPr stringRefSyntax="ExcelA1"/>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
@@ -29,6 +21,64 @@
   </authors>
   <commentList>
     <comment ref="B1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="ＭＳ Ｐゴシック"/>
+            <family val="3"/>
+            <charset val="128"/>
+          </rPr>
+          <t>Since 0.7</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="ＭＳ Ｐゴシック"/>
+            <family val="3"/>
+            <charset val="128"/>
+          </rPr>
+          <t xml:space="preserve">
+Enter valid filename. The converter will use as </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="ＭＳ Ｐゴシック"/>
+            <family val="3"/>
+            <charset val="128"/>
+          </rPr>
+          <t>output filename</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="ＭＳ Ｐゴシック"/>
+            <family val="3"/>
+            <charset val="128"/>
+          </rPr>
+          <t xml:space="preserve"> and VST </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="ＭＳ Ｐゴシック"/>
+            <family val="3"/>
+            <charset val="128"/>
+          </rPr>
+          <t>Expression Map name</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B3" authorId="0">
       <text>
         <r>
           <rPr>
@@ -48,7 +98,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="148">
   <si>
     <t>Name</t>
   </si>
@@ -480,13 +530,27 @@
   </si>
   <si>
     <t>G8 (127)</t>
+  </si>
+  <si>
+    <t>MIDI Notes(Whole)</t>
+  </si>
+  <si>
+    <t>MIDI Notes(Semi)</t>
+  </si>
+  <si>
+    <t>Example - ProductName - Patchname</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>Expression Map Name</t>
+    <phoneticPr fontId="5"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -525,8 +589,23 @@
       <name val="ＭＳ Ｐゴシック"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="ＭＳ Ｐゴシック"/>
+      <family val="3"/>
+      <charset val="128"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="ＭＳ Ｐゴシック"/>
+      <family val="3"/>
+      <charset val="128"/>
+    </font>
   </fonts>
-  <fills count="10">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -581,8 +660,20 @@
         <bgColor rgb="FFEBF1DE"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor rgb="FFB7DEE8"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -629,6 +720,19 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -638,7 +742,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -698,6 +802,30 @@
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="11" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="10" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="10" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -788,13 +916,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
+      <xdr:row>2</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>55</xdr:row>
+      <xdr:row>57</xdr:row>
       <xdr:rowOff>127000</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1101,12 +1229,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K129"/>
+  <dimension ref="A1:K131"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="F1" sqref="F1"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="18.75"/>
@@ -1121,103 +1249,71 @@
     <col min="1026" max="16384" width="8.875" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:11" ht="29.25" customHeight="1">
+      <c r="A1" s="22" t="s">
+        <v>147</v>
+      </c>
+      <c r="B1" s="26" t="s">
+        <v>146</v>
+      </c>
+      <c r="C1" s="27"/>
+    </row>
+    <row r="2" spans="1:11" ht="12" customHeight="1">
+      <c r="A2" s="21"/>
+      <c r="B2" s="20"/>
+      <c r="C2" s="20"/>
+    </row>
+    <row r="3" spans="1:11">
+      <c r="A3" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B3" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C3" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="D3" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="E3" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="12" t="s">
+      <c r="F3" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="12" t="s">
+      <c r="G3" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="13" t="s">
+      <c r="H3" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="13" t="s">
+      <c r="I3" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="14" t="s">
+      <c r="J3" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="14" t="s">
+      <c r="K3" s="14" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
-      <c r="A2" s="1" t="s">
+    <row r="4" spans="1:11">
+      <c r="A4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="15">
-        <v>0</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="E2" s="15">
-        <v>1</v>
-      </c>
-      <c r="F2" s="15"/>
-      <c r="G2" s="15"/>
-      <c r="H2" s="15"/>
-      <c r="I2" s="15"/>
-      <c r="J2" s="15"/>
-      <c r="K2" s="15"/>
-    </row>
-    <row r="3" spans="1:11">
-      <c r="A3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" s="15">
-        <v>1</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" s="15">
-        <v>1</v>
-      </c>
-      <c r="F3" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="G3" s="15">
-        <v>100</v>
-      </c>
-      <c r="H3" s="15">
-        <v>1</v>
-      </c>
-      <c r="I3" s="15">
-        <v>23</v>
-      </c>
-      <c r="J3" s="15"/>
-      <c r="K3" s="15"/>
-    </row>
-    <row r="4" spans="1:11">
-      <c r="A4" s="1"/>
       <c r="B4" s="15">
         <v>0</v>
       </c>
-      <c r="C4" s="2"/>
-      <c r="D4" s="16"/>
-      <c r="E4" s="15"/>
+      <c r="C4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="15">
+        <v>1</v>
+      </c>
       <c r="F4" s="15"/>
       <c r="G4" s="15"/>
       <c r="H4" s="15"/>
@@ -1226,25 +1322,39 @@
       <c r="K4" s="15"/>
     </row>
     <row r="5" spans="1:11">
-      <c r="A5" s="1"/>
+      <c r="A5" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="B5" s="15">
-        <v>0</v>
-      </c>
-      <c r="C5" s="2"/>
-      <c r="D5" s="16"/>
-      <c r="E5" s="15"/>
-      <c r="F5" s="15"/>
-      <c r="G5" s="15"/>
-      <c r="H5" s="15"/>
-      <c r="I5" s="15"/>
+        <v>1</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="15">
+        <v>1</v>
+      </c>
+      <c r="F5" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="G5" s="15">
+        <v>100</v>
+      </c>
+      <c r="H5" s="15">
+        <v>1</v>
+      </c>
+      <c r="I5" s="15">
+        <v>23</v>
+      </c>
       <c r="J5" s="15"/>
       <c r="K5" s="15"/>
     </row>
     <row r="6" spans="1:11">
       <c r="A6" s="1"/>
-      <c r="B6" s="15">
-        <v>0</v>
-      </c>
+      <c r="B6" s="15"/>
       <c r="C6" s="2"/>
       <c r="D6" s="16"/>
       <c r="E6" s="15"/>
@@ -1257,9 +1367,7 @@
     </row>
     <row r="7" spans="1:11">
       <c r="A7" s="1"/>
-      <c r="B7" s="15">
-        <v>0</v>
-      </c>
+      <c r="B7" s="15"/>
       <c r="C7" s="2"/>
       <c r="D7" s="16"/>
       <c r="E7" s="15"/>
@@ -1272,9 +1380,7 @@
     </row>
     <row r="8" spans="1:11">
       <c r="A8" s="1"/>
-      <c r="B8" s="15">
-        <v>0</v>
-      </c>
+      <c r="B8" s="15"/>
       <c r="C8" s="2"/>
       <c r="D8" s="16"/>
       <c r="E8" s="15"/>
@@ -1287,9 +1393,7 @@
     </row>
     <row r="9" spans="1:11">
       <c r="A9" s="1"/>
-      <c r="B9" s="15">
-        <v>0</v>
-      </c>
+      <c r="B9" s="15"/>
       <c r="C9" s="2"/>
       <c r="D9" s="16"/>
       <c r="E9" s="15"/>
@@ -1302,9 +1406,7 @@
     </row>
     <row r="10" spans="1:11">
       <c r="A10" s="1"/>
-      <c r="B10" s="15">
-        <v>0</v>
-      </c>
+      <c r="B10" s="15"/>
       <c r="C10" s="2"/>
       <c r="D10" s="16"/>
       <c r="E10" s="15"/>
@@ -1317,9 +1419,7 @@
     </row>
     <row r="11" spans="1:11">
       <c r="A11" s="1"/>
-      <c r="B11" s="15">
-        <v>0</v>
-      </c>
+      <c r="B11" s="15"/>
       <c r="C11" s="2"/>
       <c r="D11" s="16"/>
       <c r="E11" s="15"/>
@@ -1332,9 +1432,7 @@
     </row>
     <row r="12" spans="1:11">
       <c r="A12" s="1"/>
-      <c r="B12" s="15">
-        <v>0</v>
-      </c>
+      <c r="B12" s="15"/>
       <c r="C12" s="2"/>
       <c r="D12" s="16"/>
       <c r="E12" s="15"/>
@@ -1347,9 +1445,7 @@
     </row>
     <row r="13" spans="1:11">
       <c r="A13" s="1"/>
-      <c r="B13" s="15">
-        <v>0</v>
-      </c>
+      <c r="B13" s="15"/>
       <c r="C13" s="2"/>
       <c r="D13" s="16"/>
       <c r="E13" s="15"/>
@@ -1362,9 +1458,7 @@
     </row>
     <row r="14" spans="1:11">
       <c r="A14" s="1"/>
-      <c r="B14" s="15">
-        <v>0</v>
-      </c>
+      <c r="B14" s="15"/>
       <c r="C14" s="2"/>
       <c r="D14" s="16"/>
       <c r="E14" s="15"/>
@@ -1377,9 +1471,7 @@
     </row>
     <row r="15" spans="1:11">
       <c r="A15" s="1"/>
-      <c r="B15" s="15">
-        <v>0</v>
-      </c>
+      <c r="B15" s="15"/>
       <c r="C15" s="2"/>
       <c r="D15" s="16"/>
       <c r="E15" s="15"/>
@@ -1392,9 +1484,7 @@
     </row>
     <row r="16" spans="1:11">
       <c r="A16" s="1"/>
-      <c r="B16" s="15">
-        <v>0</v>
-      </c>
+      <c r="B16" s="15"/>
       <c r="C16" s="2"/>
       <c r="D16" s="16"/>
       <c r="E16" s="15"/>
@@ -1407,9 +1497,7 @@
     </row>
     <row r="17" spans="1:11">
       <c r="A17" s="1"/>
-      <c r="B17" s="15">
-        <v>0</v>
-      </c>
+      <c r="B17" s="15"/>
       <c r="C17" s="2"/>
       <c r="D17" s="16"/>
       <c r="E17" s="15"/>
@@ -1422,9 +1510,7 @@
     </row>
     <row r="18" spans="1:11">
       <c r="A18" s="1"/>
-      <c r="B18" s="15">
-        <v>0</v>
-      </c>
+      <c r="B18" s="15"/>
       <c r="C18" s="2"/>
       <c r="D18" s="16"/>
       <c r="E18" s="15"/>
@@ -1437,9 +1523,7 @@
     </row>
     <row r="19" spans="1:11">
       <c r="A19" s="1"/>
-      <c r="B19" s="15">
-        <v>0</v>
-      </c>
+      <c r="B19" s="15"/>
       <c r="C19" s="2"/>
       <c r="D19" s="16"/>
       <c r="E19" s="15"/>
@@ -1452,9 +1536,7 @@
     </row>
     <row r="20" spans="1:11">
       <c r="A20" s="1"/>
-      <c r="B20" s="15">
-        <v>0</v>
-      </c>
+      <c r="B20" s="15"/>
       <c r="C20" s="2"/>
       <c r="D20" s="16"/>
       <c r="E20" s="15"/>
@@ -1467,9 +1549,7 @@
     </row>
     <row r="21" spans="1:11">
       <c r="A21" s="1"/>
-      <c r="B21" s="15">
-        <v>0</v>
-      </c>
+      <c r="B21" s="15"/>
       <c r="C21" s="2"/>
       <c r="D21" s="16"/>
       <c r="E21" s="15"/>
@@ -1482,9 +1562,7 @@
     </row>
     <row r="22" spans="1:11">
       <c r="A22" s="1"/>
-      <c r="B22" s="15">
-        <v>0</v>
-      </c>
+      <c r="B22" s="15"/>
       <c r="C22" s="2"/>
       <c r="D22" s="16"/>
       <c r="E22" s="15"/>
@@ -1497,9 +1575,7 @@
     </row>
     <row r="23" spans="1:11">
       <c r="A23" s="1"/>
-      <c r="B23" s="15">
-        <v>0</v>
-      </c>
+      <c r="B23" s="15"/>
       <c r="C23" s="2"/>
       <c r="D23" s="16"/>
       <c r="E23" s="15"/>
@@ -1512,9 +1588,7 @@
     </row>
     <row r="24" spans="1:11">
       <c r="A24" s="1"/>
-      <c r="B24" s="15">
-        <v>0</v>
-      </c>
+      <c r="B24" s="15"/>
       <c r="C24" s="2"/>
       <c r="D24" s="16"/>
       <c r="E24" s="15"/>
@@ -1527,9 +1601,7 @@
     </row>
     <row r="25" spans="1:11">
       <c r="A25" s="1"/>
-      <c r="B25" s="15">
-        <v>0</v>
-      </c>
+      <c r="B25" s="15"/>
       <c r="C25" s="2"/>
       <c r="D25" s="16"/>
       <c r="E25" s="15"/>
@@ -1542,9 +1614,7 @@
     </row>
     <row r="26" spans="1:11">
       <c r="A26" s="1"/>
-      <c r="B26" s="15">
-        <v>0</v>
-      </c>
+      <c r="B26" s="15"/>
       <c r="C26" s="2"/>
       <c r="D26" s="16"/>
       <c r="E26" s="15"/>
@@ -1557,9 +1627,7 @@
     </row>
     <row r="27" spans="1:11">
       <c r="A27" s="1"/>
-      <c r="B27" s="15">
-        <v>0</v>
-      </c>
+      <c r="B27" s="15"/>
       <c r="C27" s="2"/>
       <c r="D27" s="16"/>
       <c r="E27" s="15"/>
@@ -1572,9 +1640,7 @@
     </row>
     <row r="28" spans="1:11">
       <c r="A28" s="1"/>
-      <c r="B28" s="15">
-        <v>0</v>
-      </c>
+      <c r="B28" s="15"/>
       <c r="C28" s="2"/>
       <c r="D28" s="16"/>
       <c r="E28" s="15"/>
@@ -1587,9 +1653,7 @@
     </row>
     <row r="29" spans="1:11">
       <c r="A29" s="1"/>
-      <c r="B29" s="15">
-        <v>0</v>
-      </c>
+      <c r="B29" s="15"/>
       <c r="C29" s="2"/>
       <c r="D29" s="16"/>
       <c r="E29" s="15"/>
@@ -1602,9 +1666,7 @@
     </row>
     <row r="30" spans="1:11">
       <c r="A30" s="1"/>
-      <c r="B30" s="15">
-        <v>0</v>
-      </c>
+      <c r="B30" s="15"/>
       <c r="C30" s="2"/>
       <c r="D30" s="16"/>
       <c r="E30" s="15"/>
@@ -1617,9 +1679,7 @@
     </row>
     <row r="31" spans="1:11">
       <c r="A31" s="1"/>
-      <c r="B31" s="15">
-        <v>0</v>
-      </c>
+      <c r="B31" s="15"/>
       <c r="C31" s="2"/>
       <c r="D31" s="16"/>
       <c r="E31" s="15"/>
@@ -1632,9 +1692,7 @@
     </row>
     <row r="32" spans="1:11">
       <c r="A32" s="1"/>
-      <c r="B32" s="15">
-        <v>0</v>
-      </c>
+      <c r="B32" s="15"/>
       <c r="C32" s="2"/>
       <c r="D32" s="16"/>
       <c r="E32" s="15"/>
@@ -1647,9 +1705,7 @@
     </row>
     <row r="33" spans="1:11">
       <c r="A33" s="1"/>
-      <c r="B33" s="15">
-        <v>0</v>
-      </c>
+      <c r="B33" s="15"/>
       <c r="C33" s="2"/>
       <c r="D33" s="16"/>
       <c r="E33" s="15"/>
@@ -1662,9 +1718,7 @@
     </row>
     <row r="34" spans="1:11">
       <c r="A34" s="1"/>
-      <c r="B34" s="15">
-        <v>0</v>
-      </c>
+      <c r="B34" s="15"/>
       <c r="C34" s="2"/>
       <c r="D34" s="16"/>
       <c r="E34" s="15"/>
@@ -1677,9 +1731,7 @@
     </row>
     <row r="35" spans="1:11">
       <c r="A35" s="1"/>
-      <c r="B35" s="15">
-        <v>0</v>
-      </c>
+      <c r="B35" s="15"/>
       <c r="C35" s="2"/>
       <c r="D35" s="16"/>
       <c r="E35" s="15"/>
@@ -1692,9 +1744,7 @@
     </row>
     <row r="36" spans="1:11">
       <c r="A36" s="1"/>
-      <c r="B36" s="15">
-        <v>0</v>
-      </c>
+      <c r="B36" s="15"/>
       <c r="C36" s="2"/>
       <c r="D36" s="16"/>
       <c r="E36" s="15"/>
@@ -1707,9 +1757,7 @@
     </row>
     <row r="37" spans="1:11">
       <c r="A37" s="1"/>
-      <c r="B37" s="15">
-        <v>0</v>
-      </c>
+      <c r="B37" s="15"/>
       <c r="C37" s="2"/>
       <c r="D37" s="16"/>
       <c r="E37" s="15"/>
@@ -1722,9 +1770,7 @@
     </row>
     <row r="38" spans="1:11">
       <c r="A38" s="1"/>
-      <c r="B38" s="15">
-        <v>0</v>
-      </c>
+      <c r="B38" s="15"/>
       <c r="C38" s="2"/>
       <c r="D38" s="16"/>
       <c r="E38" s="15"/>
@@ -1737,9 +1783,7 @@
     </row>
     <row r="39" spans="1:11">
       <c r="A39" s="1"/>
-      <c r="B39" s="15">
-        <v>0</v>
-      </c>
+      <c r="B39" s="15"/>
       <c r="C39" s="2"/>
       <c r="D39" s="16"/>
       <c r="E39" s="15"/>
@@ -1752,9 +1796,7 @@
     </row>
     <row r="40" spans="1:11">
       <c r="A40" s="1"/>
-      <c r="B40" s="15">
-        <v>0</v>
-      </c>
+      <c r="B40" s="15"/>
       <c r="C40" s="2"/>
       <c r="D40" s="16"/>
       <c r="E40" s="15"/>
@@ -1767,9 +1809,7 @@
     </row>
     <row r="41" spans="1:11">
       <c r="A41" s="1"/>
-      <c r="B41" s="15">
-        <v>0</v>
-      </c>
+      <c r="B41" s="15"/>
       <c r="C41" s="2"/>
       <c r="D41" s="16"/>
       <c r="E41" s="15"/>
@@ -1782,9 +1822,7 @@
     </row>
     <row r="42" spans="1:11">
       <c r="A42" s="1"/>
-      <c r="B42" s="15">
-        <v>0</v>
-      </c>
+      <c r="B42" s="15"/>
       <c r="C42" s="2"/>
       <c r="D42" s="16"/>
       <c r="E42" s="15"/>
@@ -1797,9 +1835,7 @@
     </row>
     <row r="43" spans="1:11">
       <c r="A43" s="1"/>
-      <c r="B43" s="15">
-        <v>0</v>
-      </c>
+      <c r="B43" s="15"/>
       <c r="C43" s="2"/>
       <c r="D43" s="16"/>
       <c r="E43" s="15"/>
@@ -1812,9 +1848,7 @@
     </row>
     <row r="44" spans="1:11">
       <c r="A44" s="1"/>
-      <c r="B44" s="15">
-        <v>0</v>
-      </c>
+      <c r="B44" s="15"/>
       <c r="C44" s="2"/>
       <c r="D44" s="16"/>
       <c r="E44" s="15"/>
@@ -1827,9 +1861,7 @@
     </row>
     <row r="45" spans="1:11">
       <c r="A45" s="1"/>
-      <c r="B45" s="15">
-        <v>0</v>
-      </c>
+      <c r="B45" s="15"/>
       <c r="C45" s="2"/>
       <c r="D45" s="16"/>
       <c r="E45" s="15"/>
@@ -1842,9 +1874,7 @@
     </row>
     <row r="46" spans="1:11">
       <c r="A46" s="1"/>
-      <c r="B46" s="15">
-        <v>0</v>
-      </c>
+      <c r="B46" s="15"/>
       <c r="C46" s="2"/>
       <c r="D46" s="16"/>
       <c r="E46" s="15"/>
@@ -1857,9 +1887,7 @@
     </row>
     <row r="47" spans="1:11">
       <c r="A47" s="1"/>
-      <c r="B47" s="15">
-        <v>0</v>
-      </c>
+      <c r="B47" s="15"/>
       <c r="C47" s="2"/>
       <c r="D47" s="16"/>
       <c r="E47" s="15"/>
@@ -1872,9 +1900,7 @@
     </row>
     <row r="48" spans="1:11">
       <c r="A48" s="1"/>
-      <c r="B48" s="15">
-        <v>0</v>
-      </c>
+      <c r="B48" s="15"/>
       <c r="C48" s="2"/>
       <c r="D48" s="16"/>
       <c r="E48" s="15"/>
@@ -1887,9 +1913,7 @@
     </row>
     <row r="49" spans="1:11">
       <c r="A49" s="1"/>
-      <c r="B49" s="15">
-        <v>0</v>
-      </c>
+      <c r="B49" s="15"/>
       <c r="C49" s="2"/>
       <c r="D49" s="16"/>
       <c r="E49" s="15"/>
@@ -1902,9 +1926,7 @@
     </row>
     <row r="50" spans="1:11">
       <c r="A50" s="1"/>
-      <c r="B50" s="15">
-        <v>0</v>
-      </c>
+      <c r="B50" s="15"/>
       <c r="C50" s="2"/>
       <c r="D50" s="16"/>
       <c r="E50" s="15"/>
@@ -1917,9 +1939,7 @@
     </row>
     <row r="51" spans="1:11">
       <c r="A51" s="1"/>
-      <c r="B51" s="15">
-        <v>0</v>
-      </c>
+      <c r="B51" s="15"/>
       <c r="C51" s="2"/>
       <c r="D51" s="16"/>
       <c r="E51" s="15"/>
@@ -1932,9 +1952,7 @@
     </row>
     <row r="52" spans="1:11">
       <c r="A52" s="1"/>
-      <c r="B52" s="15">
-        <v>0</v>
-      </c>
+      <c r="B52" s="15"/>
       <c r="C52" s="2"/>
       <c r="D52" s="16"/>
       <c r="E52" s="15"/>
@@ -1947,9 +1965,7 @@
     </row>
     <row r="53" spans="1:11">
       <c r="A53" s="1"/>
-      <c r="B53" s="15">
-        <v>0</v>
-      </c>
+      <c r="B53" s="15"/>
       <c r="C53" s="2"/>
       <c r="D53" s="16"/>
       <c r="E53" s="15"/>
@@ -1962,9 +1978,7 @@
     </row>
     <row r="54" spans="1:11">
       <c r="A54" s="1"/>
-      <c r="B54" s="15">
-        <v>0</v>
-      </c>
+      <c r="B54" s="15"/>
       <c r="C54" s="2"/>
       <c r="D54" s="16"/>
       <c r="E54" s="15"/>
@@ -1977,9 +1991,7 @@
     </row>
     <row r="55" spans="1:11">
       <c r="A55" s="1"/>
-      <c r="B55" s="15">
-        <v>0</v>
-      </c>
+      <c r="B55" s="15"/>
       <c r="C55" s="2"/>
       <c r="D55" s="16"/>
       <c r="E55" s="15"/>
@@ -1992,9 +2004,7 @@
     </row>
     <row r="56" spans="1:11">
       <c r="A56" s="1"/>
-      <c r="B56" s="15">
-        <v>0</v>
-      </c>
+      <c r="B56" s="15"/>
       <c r="C56" s="2"/>
       <c r="D56" s="16"/>
       <c r="E56" s="15"/>
@@ -2007,9 +2017,7 @@
     </row>
     <row r="57" spans="1:11">
       <c r="A57" s="1"/>
-      <c r="B57" s="15">
-        <v>0</v>
-      </c>
+      <c r="B57" s="15"/>
       <c r="C57" s="2"/>
       <c r="D57" s="16"/>
       <c r="E57" s="15"/>
@@ -2022,9 +2030,7 @@
     </row>
     <row r="58" spans="1:11">
       <c r="A58" s="1"/>
-      <c r="B58" s="15">
-        <v>0</v>
-      </c>
+      <c r="B58" s="15"/>
       <c r="C58" s="2"/>
       <c r="D58" s="16"/>
       <c r="E58" s="15"/>
@@ -2037,9 +2043,7 @@
     </row>
     <row r="59" spans="1:11">
       <c r="A59" s="1"/>
-      <c r="B59" s="15">
-        <v>0</v>
-      </c>
+      <c r="B59" s="15"/>
       <c r="C59" s="2"/>
       <c r="D59" s="16"/>
       <c r="E59" s="15"/>
@@ -2052,9 +2056,7 @@
     </row>
     <row r="60" spans="1:11">
       <c r="A60" s="1"/>
-      <c r="B60" s="15">
-        <v>0</v>
-      </c>
+      <c r="B60" s="15"/>
       <c r="C60" s="2"/>
       <c r="D60" s="16"/>
       <c r="E60" s="15"/>
@@ -2067,9 +2069,7 @@
     </row>
     <row r="61" spans="1:11">
       <c r="A61" s="1"/>
-      <c r="B61" s="15">
-        <v>0</v>
-      </c>
+      <c r="B61" s="15"/>
       <c r="C61" s="2"/>
       <c r="D61" s="16"/>
       <c r="E61" s="15"/>
@@ -2082,9 +2082,7 @@
     </row>
     <row r="62" spans="1:11">
       <c r="A62" s="1"/>
-      <c r="B62" s="15">
-        <v>0</v>
-      </c>
+      <c r="B62" s="15"/>
       <c r="C62" s="2"/>
       <c r="D62" s="16"/>
       <c r="E62" s="15"/>
@@ -2097,9 +2095,7 @@
     </row>
     <row r="63" spans="1:11">
       <c r="A63" s="1"/>
-      <c r="B63" s="15">
-        <v>0</v>
-      </c>
+      <c r="B63" s="15"/>
       <c r="C63" s="2"/>
       <c r="D63" s="16"/>
       <c r="E63" s="15"/>
@@ -2112,9 +2108,7 @@
     </row>
     <row r="64" spans="1:11">
       <c r="A64" s="1"/>
-      <c r="B64" s="15">
-        <v>0</v>
-      </c>
+      <c r="B64" s="15"/>
       <c r="C64" s="2"/>
       <c r="D64" s="16"/>
       <c r="E64" s="15"/>
@@ -2127,9 +2121,7 @@
     </row>
     <row r="65" spans="1:11">
       <c r="A65" s="1"/>
-      <c r="B65" s="15">
-        <v>0</v>
-      </c>
+      <c r="B65" s="15"/>
       <c r="C65" s="2"/>
       <c r="D65" s="16"/>
       <c r="E65" s="15"/>
@@ -2142,9 +2134,7 @@
     </row>
     <row r="66" spans="1:11">
       <c r="A66" s="1"/>
-      <c r="B66" s="15">
-        <v>0</v>
-      </c>
+      <c r="B66" s="15"/>
       <c r="C66" s="2"/>
       <c r="D66" s="16"/>
       <c r="E66" s="15"/>
@@ -2157,9 +2147,7 @@
     </row>
     <row r="67" spans="1:11">
       <c r="A67" s="1"/>
-      <c r="B67" s="15">
-        <v>0</v>
-      </c>
+      <c r="B67" s="15"/>
       <c r="C67" s="2"/>
       <c r="D67" s="16"/>
       <c r="E67" s="15"/>
@@ -2172,9 +2160,7 @@
     </row>
     <row r="68" spans="1:11">
       <c r="A68" s="1"/>
-      <c r="B68" s="15">
-        <v>0</v>
-      </c>
+      <c r="B68" s="15"/>
       <c r="C68" s="2"/>
       <c r="D68" s="16"/>
       <c r="E68" s="15"/>
@@ -2187,9 +2173,7 @@
     </row>
     <row r="69" spans="1:11">
       <c r="A69" s="1"/>
-      <c r="B69" s="15">
-        <v>0</v>
-      </c>
+      <c r="B69" s="15"/>
       <c r="C69" s="2"/>
       <c r="D69" s="16"/>
       <c r="E69" s="15"/>
@@ -2202,9 +2186,7 @@
     </row>
     <row r="70" spans="1:11">
       <c r="A70" s="1"/>
-      <c r="B70" s="15">
-        <v>0</v>
-      </c>
+      <c r="B70" s="15"/>
       <c r="C70" s="2"/>
       <c r="D70" s="16"/>
       <c r="E70" s="15"/>
@@ -2217,9 +2199,7 @@
     </row>
     <row r="71" spans="1:11">
       <c r="A71" s="1"/>
-      <c r="B71" s="15">
-        <v>0</v>
-      </c>
+      <c r="B71" s="15"/>
       <c r="C71" s="2"/>
       <c r="D71" s="16"/>
       <c r="E71" s="15"/>
@@ -2232,9 +2212,7 @@
     </row>
     <row r="72" spans="1:11">
       <c r="A72" s="1"/>
-      <c r="B72" s="15">
-        <v>0</v>
-      </c>
+      <c r="B72" s="15"/>
       <c r="C72" s="2"/>
       <c r="D72" s="16"/>
       <c r="E72" s="15"/>
@@ -2247,9 +2225,7 @@
     </row>
     <row r="73" spans="1:11">
       <c r="A73" s="1"/>
-      <c r="B73" s="15">
-        <v>0</v>
-      </c>
+      <c r="B73" s="15"/>
       <c r="C73" s="2"/>
       <c r="D73" s="16"/>
       <c r="E73" s="15"/>
@@ -2262,9 +2238,7 @@
     </row>
     <row r="74" spans="1:11">
       <c r="A74" s="1"/>
-      <c r="B74" s="15">
-        <v>0</v>
-      </c>
+      <c r="B74" s="15"/>
       <c r="C74" s="2"/>
       <c r="D74" s="16"/>
       <c r="E74" s="15"/>
@@ -2277,9 +2251,7 @@
     </row>
     <row r="75" spans="1:11">
       <c r="A75" s="1"/>
-      <c r="B75" s="15">
-        <v>0</v>
-      </c>
+      <c r="B75" s="15"/>
       <c r="C75" s="2"/>
       <c r="D75" s="16"/>
       <c r="E75" s="15"/>
@@ -2292,9 +2264,7 @@
     </row>
     <row r="76" spans="1:11">
       <c r="A76" s="1"/>
-      <c r="B76" s="15">
-        <v>0</v>
-      </c>
+      <c r="B76" s="15"/>
       <c r="C76" s="2"/>
       <c r="D76" s="16"/>
       <c r="E76" s="15"/>
@@ -2307,9 +2277,7 @@
     </row>
     <row r="77" spans="1:11">
       <c r="A77" s="1"/>
-      <c r="B77" s="15">
-        <v>0</v>
-      </c>
+      <c r="B77" s="15"/>
       <c r="C77" s="2"/>
       <c r="D77" s="16"/>
       <c r="E77" s="15"/>
@@ -2322,9 +2290,7 @@
     </row>
     <row r="78" spans="1:11">
       <c r="A78" s="1"/>
-      <c r="B78" s="15">
-        <v>0</v>
-      </c>
+      <c r="B78" s="15"/>
       <c r="C78" s="2"/>
       <c r="D78" s="16"/>
       <c r="E78" s="15"/>
@@ -2337,9 +2303,7 @@
     </row>
     <row r="79" spans="1:11">
       <c r="A79" s="1"/>
-      <c r="B79" s="15">
-        <v>0</v>
-      </c>
+      <c r="B79" s="15"/>
       <c r="C79" s="2"/>
       <c r="D79" s="16"/>
       <c r="E79" s="15"/>
@@ -2352,9 +2316,7 @@
     </row>
     <row r="80" spans="1:11">
       <c r="A80" s="1"/>
-      <c r="B80" s="15">
-        <v>0</v>
-      </c>
+      <c r="B80" s="15"/>
       <c r="C80" s="2"/>
       <c r="D80" s="16"/>
       <c r="E80" s="15"/>
@@ -2367,9 +2329,7 @@
     </row>
     <row r="81" spans="1:11">
       <c r="A81" s="1"/>
-      <c r="B81" s="15">
-        <v>0</v>
-      </c>
+      <c r="B81" s="15"/>
       <c r="C81" s="2"/>
       <c r="D81" s="16"/>
       <c r="E81" s="15"/>
@@ -2382,9 +2342,7 @@
     </row>
     <row r="82" spans="1:11">
       <c r="A82" s="1"/>
-      <c r="B82" s="15">
-        <v>0</v>
-      </c>
+      <c r="B82" s="15"/>
       <c r="C82" s="2"/>
       <c r="D82" s="16"/>
       <c r="E82" s="15"/>
@@ -2397,9 +2355,7 @@
     </row>
     <row r="83" spans="1:11">
       <c r="A83" s="1"/>
-      <c r="B83" s="15">
-        <v>0</v>
-      </c>
+      <c r="B83" s="15"/>
       <c r="C83" s="2"/>
       <c r="D83" s="16"/>
       <c r="E83" s="15"/>
@@ -2412,9 +2368,7 @@
     </row>
     <row r="84" spans="1:11">
       <c r="A84" s="1"/>
-      <c r="B84" s="15">
-        <v>0</v>
-      </c>
+      <c r="B84" s="15"/>
       <c r="C84" s="2"/>
       <c r="D84" s="16"/>
       <c r="E84" s="15"/>
@@ -2427,9 +2381,7 @@
     </row>
     <row r="85" spans="1:11">
       <c r="A85" s="1"/>
-      <c r="B85" s="15">
-        <v>0</v>
-      </c>
+      <c r="B85" s="15"/>
       <c r="C85" s="2"/>
       <c r="D85" s="16"/>
       <c r="E85" s="15"/>
@@ -2442,9 +2394,7 @@
     </row>
     <row r="86" spans="1:11">
       <c r="A86" s="1"/>
-      <c r="B86" s="15">
-        <v>0</v>
-      </c>
+      <c r="B86" s="15"/>
       <c r="C86" s="2"/>
       <c r="D86" s="16"/>
       <c r="E86" s="15"/>
@@ -2457,9 +2407,7 @@
     </row>
     <row r="87" spans="1:11">
       <c r="A87" s="1"/>
-      <c r="B87" s="15">
-        <v>0</v>
-      </c>
+      <c r="B87" s="15"/>
       <c r="C87" s="2"/>
       <c r="D87" s="16"/>
       <c r="E87" s="15"/>
@@ -2472,9 +2420,7 @@
     </row>
     <row r="88" spans="1:11">
       <c r="A88" s="1"/>
-      <c r="B88" s="15">
-        <v>0</v>
-      </c>
+      <c r="B88" s="15"/>
       <c r="C88" s="2"/>
       <c r="D88" s="16"/>
       <c r="E88" s="15"/>
@@ -2487,9 +2433,7 @@
     </row>
     <row r="89" spans="1:11">
       <c r="A89" s="1"/>
-      <c r="B89" s="15">
-        <v>0</v>
-      </c>
+      <c r="B89" s="15"/>
       <c r="C89" s="2"/>
       <c r="D89" s="16"/>
       <c r="E89" s="15"/>
@@ -2502,9 +2446,7 @@
     </row>
     <row r="90" spans="1:11">
       <c r="A90" s="1"/>
-      <c r="B90" s="15">
-        <v>0</v>
-      </c>
+      <c r="B90" s="15"/>
       <c r="C90" s="2"/>
       <c r="D90" s="16"/>
       <c r="E90" s="15"/>
@@ -2517,9 +2459,7 @@
     </row>
     <row r="91" spans="1:11">
       <c r="A91" s="1"/>
-      <c r="B91" s="15">
-        <v>0</v>
-      </c>
+      <c r="B91" s="15"/>
       <c r="C91" s="2"/>
       <c r="D91" s="16"/>
       <c r="E91" s="15"/>
@@ -2532,9 +2472,7 @@
     </row>
     <row r="92" spans="1:11">
       <c r="A92" s="1"/>
-      <c r="B92" s="15">
-        <v>0</v>
-      </c>
+      <c r="B92" s="15"/>
       <c r="C92" s="2"/>
       <c r="D92" s="16"/>
       <c r="E92" s="15"/>
@@ -2547,9 +2485,7 @@
     </row>
     <row r="93" spans="1:11">
       <c r="A93" s="1"/>
-      <c r="B93" s="15">
-        <v>0</v>
-      </c>
+      <c r="B93" s="15"/>
       <c r="C93" s="2"/>
       <c r="D93" s="16"/>
       <c r="E93" s="15"/>
@@ -2562,9 +2498,7 @@
     </row>
     <row r="94" spans="1:11">
       <c r="A94" s="1"/>
-      <c r="B94" s="15">
-        <v>0</v>
-      </c>
+      <c r="B94" s="15"/>
       <c r="C94" s="2"/>
       <c r="D94" s="16"/>
       <c r="E94" s="15"/>
@@ -2577,9 +2511,7 @@
     </row>
     <row r="95" spans="1:11">
       <c r="A95" s="1"/>
-      <c r="B95" s="15">
-        <v>0</v>
-      </c>
+      <c r="B95" s="15"/>
       <c r="C95" s="2"/>
       <c r="D95" s="16"/>
       <c r="E95" s="15"/>
@@ -2592,9 +2524,7 @@
     </row>
     <row r="96" spans="1:11">
       <c r="A96" s="1"/>
-      <c r="B96" s="15">
-        <v>0</v>
-      </c>
+      <c r="B96" s="15"/>
       <c r="C96" s="2"/>
       <c r="D96" s="16"/>
       <c r="E96" s="15"/>
@@ -2607,9 +2537,7 @@
     </row>
     <row r="97" spans="1:11">
       <c r="A97" s="1"/>
-      <c r="B97" s="15">
-        <v>0</v>
-      </c>
+      <c r="B97" s="15"/>
       <c r="C97" s="2"/>
       <c r="D97" s="16"/>
       <c r="E97" s="15"/>
@@ -2622,9 +2550,7 @@
     </row>
     <row r="98" spans="1:11">
       <c r="A98" s="1"/>
-      <c r="B98" s="15">
-        <v>0</v>
-      </c>
+      <c r="B98" s="15"/>
       <c r="C98" s="2"/>
       <c r="D98" s="16"/>
       <c r="E98" s="15"/>
@@ -2637,9 +2563,7 @@
     </row>
     <row r="99" spans="1:11">
       <c r="A99" s="1"/>
-      <c r="B99" s="15">
-        <v>0</v>
-      </c>
+      <c r="B99" s="15"/>
       <c r="C99" s="2"/>
       <c r="D99" s="16"/>
       <c r="E99" s="15"/>
@@ -2652,9 +2576,7 @@
     </row>
     <row r="100" spans="1:11">
       <c r="A100" s="1"/>
-      <c r="B100" s="15">
-        <v>0</v>
-      </c>
+      <c r="B100" s="15"/>
       <c r="C100" s="2"/>
       <c r="D100" s="16"/>
       <c r="E100" s="15"/>
@@ -2667,9 +2589,7 @@
     </row>
     <row r="101" spans="1:11">
       <c r="A101" s="1"/>
-      <c r="B101" s="15">
-        <v>0</v>
-      </c>
+      <c r="B101" s="15"/>
       <c r="C101" s="2"/>
       <c r="D101" s="16"/>
       <c r="E101" s="15"/>
@@ -2682,9 +2602,7 @@
     </row>
     <row r="102" spans="1:11">
       <c r="A102" s="1"/>
-      <c r="B102" s="15">
-        <v>0</v>
-      </c>
+      <c r="B102" s="15"/>
       <c r="C102" s="2"/>
       <c r="D102" s="16"/>
       <c r="E102" s="15"/>
@@ -2697,9 +2615,7 @@
     </row>
     <row r="103" spans="1:11">
       <c r="A103" s="1"/>
-      <c r="B103" s="15">
-        <v>0</v>
-      </c>
+      <c r="B103" s="15"/>
       <c r="C103" s="2"/>
       <c r="D103" s="16"/>
       <c r="E103" s="15"/>
@@ -2712,9 +2628,7 @@
     </row>
     <row r="104" spans="1:11">
       <c r="A104" s="1"/>
-      <c r="B104" s="15">
-        <v>0</v>
-      </c>
+      <c r="B104" s="15"/>
       <c r="C104" s="2"/>
       <c r="D104" s="16"/>
       <c r="E104" s="15"/>
@@ -2727,9 +2641,7 @@
     </row>
     <row r="105" spans="1:11">
       <c r="A105" s="1"/>
-      <c r="B105" s="15">
-        <v>0</v>
-      </c>
+      <c r="B105" s="15"/>
       <c r="C105" s="2"/>
       <c r="D105" s="16"/>
       <c r="E105" s="15"/>
@@ -2742,9 +2654,7 @@
     </row>
     <row r="106" spans="1:11">
       <c r="A106" s="1"/>
-      <c r="B106" s="15">
-        <v>0</v>
-      </c>
+      <c r="B106" s="15"/>
       <c r="C106" s="2"/>
       <c r="D106" s="16"/>
       <c r="E106" s="15"/>
@@ -2757,9 +2667,7 @@
     </row>
     <row r="107" spans="1:11">
       <c r="A107" s="1"/>
-      <c r="B107" s="15">
-        <v>0</v>
-      </c>
+      <c r="B107" s="15"/>
       <c r="C107" s="2"/>
       <c r="D107" s="16"/>
       <c r="E107" s="15"/>
@@ -2772,9 +2680,7 @@
     </row>
     <row r="108" spans="1:11">
       <c r="A108" s="1"/>
-      <c r="B108" s="15">
-        <v>0</v>
-      </c>
+      <c r="B108" s="15"/>
       <c r="C108" s="2"/>
       <c r="D108" s="16"/>
       <c r="E108" s="15"/>
@@ -2787,9 +2693,7 @@
     </row>
     <row r="109" spans="1:11">
       <c r="A109" s="1"/>
-      <c r="B109" s="15">
-        <v>0</v>
-      </c>
+      <c r="B109" s="15"/>
       <c r="C109" s="2"/>
       <c r="D109" s="16"/>
       <c r="E109" s="15"/>
@@ -2802,9 +2706,7 @@
     </row>
     <row r="110" spans="1:11">
       <c r="A110" s="1"/>
-      <c r="B110" s="15">
-        <v>0</v>
-      </c>
+      <c r="B110" s="15"/>
       <c r="C110" s="2"/>
       <c r="D110" s="16"/>
       <c r="E110" s="15"/>
@@ -2817,9 +2719,7 @@
     </row>
     <row r="111" spans="1:11">
       <c r="A111" s="1"/>
-      <c r="B111" s="15">
-        <v>0</v>
-      </c>
+      <c r="B111" s="15"/>
       <c r="C111" s="2"/>
       <c r="D111" s="16"/>
       <c r="E111" s="15"/>
@@ -2832,9 +2732,7 @@
     </row>
     <row r="112" spans="1:11">
       <c r="A112" s="1"/>
-      <c r="B112" s="15">
-        <v>0</v>
-      </c>
+      <c r="B112" s="15"/>
       <c r="C112" s="2"/>
       <c r="D112" s="16"/>
       <c r="E112" s="15"/>
@@ -2847,9 +2745,7 @@
     </row>
     <row r="113" spans="1:11">
       <c r="A113" s="1"/>
-      <c r="B113" s="15">
-        <v>0</v>
-      </c>
+      <c r="B113" s="15"/>
       <c r="C113" s="2"/>
       <c r="D113" s="16"/>
       <c r="E113" s="15"/>
@@ -2862,9 +2758,7 @@
     </row>
     <row r="114" spans="1:11">
       <c r="A114" s="1"/>
-      <c r="B114" s="15">
-        <v>0</v>
-      </c>
+      <c r="B114" s="15"/>
       <c r="C114" s="2"/>
       <c r="D114" s="16"/>
       <c r="E114" s="15"/>
@@ -2877,9 +2771,7 @@
     </row>
     <row r="115" spans="1:11">
       <c r="A115" s="1"/>
-      <c r="B115" s="15">
-        <v>0</v>
-      </c>
+      <c r="B115" s="15"/>
       <c r="C115" s="2"/>
       <c r="D115" s="16"/>
       <c r="E115" s="15"/>
@@ -2892,9 +2784,7 @@
     </row>
     <row r="116" spans="1:11">
       <c r="A116" s="1"/>
-      <c r="B116" s="15">
-        <v>0</v>
-      </c>
+      <c r="B116" s="15"/>
       <c r="C116" s="2"/>
       <c r="D116" s="16"/>
       <c r="E116" s="15"/>
@@ -2907,9 +2797,7 @@
     </row>
     <row r="117" spans="1:11">
       <c r="A117" s="1"/>
-      <c r="B117" s="15">
-        <v>0</v>
-      </c>
+      <c r="B117" s="15"/>
       <c r="C117" s="2"/>
       <c r="D117" s="16"/>
       <c r="E117" s="15"/>
@@ -2922,9 +2810,7 @@
     </row>
     <row r="118" spans="1:11">
       <c r="A118" s="1"/>
-      <c r="B118" s="15">
-        <v>0</v>
-      </c>
+      <c r="B118" s="15"/>
       <c r="C118" s="2"/>
       <c r="D118" s="16"/>
       <c r="E118" s="15"/>
@@ -2937,9 +2823,7 @@
     </row>
     <row r="119" spans="1:11">
       <c r="A119" s="1"/>
-      <c r="B119" s="15">
-        <v>0</v>
-      </c>
+      <c r="B119" s="15"/>
       <c r="C119" s="2"/>
       <c r="D119" s="16"/>
       <c r="E119" s="15"/>
@@ -2952,9 +2836,7 @@
     </row>
     <row r="120" spans="1:11">
       <c r="A120" s="1"/>
-      <c r="B120" s="15">
-        <v>0</v>
-      </c>
+      <c r="B120" s="15"/>
       <c r="C120" s="2"/>
       <c r="D120" s="16"/>
       <c r="E120" s="15"/>
@@ -2967,9 +2849,7 @@
     </row>
     <row r="121" spans="1:11">
       <c r="A121" s="1"/>
-      <c r="B121" s="15">
-        <v>0</v>
-      </c>
+      <c r="B121" s="15"/>
       <c r="C121" s="2"/>
       <c r="D121" s="16"/>
       <c r="E121" s="15"/>
@@ -2982,9 +2862,7 @@
     </row>
     <row r="122" spans="1:11">
       <c r="A122" s="1"/>
-      <c r="B122" s="15">
-        <v>0</v>
-      </c>
+      <c r="B122" s="15"/>
       <c r="C122" s="2"/>
       <c r="D122" s="16"/>
       <c r="E122" s="15"/>
@@ -2997,9 +2875,7 @@
     </row>
     <row r="123" spans="1:11">
       <c r="A123" s="1"/>
-      <c r="B123" s="15">
-        <v>0</v>
-      </c>
+      <c r="B123" s="15"/>
       <c r="C123" s="2"/>
       <c r="D123" s="16"/>
       <c r="E123" s="15"/>
@@ -3012,9 +2888,7 @@
     </row>
     <row r="124" spans="1:11">
       <c r="A124" s="1"/>
-      <c r="B124" s="15">
-        <v>0</v>
-      </c>
+      <c r="B124" s="15"/>
       <c r="C124" s="2"/>
       <c r="D124" s="16"/>
       <c r="E124" s="15"/>
@@ -3027,9 +2901,7 @@
     </row>
     <row r="125" spans="1:11">
       <c r="A125" s="1"/>
-      <c r="B125" s="15">
-        <v>0</v>
-      </c>
+      <c r="B125" s="15"/>
       <c r="C125" s="2"/>
       <c r="D125" s="16"/>
       <c r="E125" s="15"/>
@@ -3042,9 +2914,7 @@
     </row>
     <row r="126" spans="1:11">
       <c r="A126" s="1"/>
-      <c r="B126" s="15">
-        <v>0</v>
-      </c>
+      <c r="B126" s="15"/>
       <c r="C126" s="2"/>
       <c r="D126" s="16"/>
       <c r="E126" s="15"/>
@@ -3057,9 +2927,7 @@
     </row>
     <row r="127" spans="1:11">
       <c r="A127" s="1"/>
-      <c r="B127" s="15">
-        <v>0</v>
-      </c>
+      <c r="B127" s="15"/>
       <c r="C127" s="2"/>
       <c r="D127" s="16"/>
       <c r="E127" s="15"/>
@@ -3072,9 +2940,7 @@
     </row>
     <row r="128" spans="1:11">
       <c r="A128" s="1"/>
-      <c r="B128" s="15">
-        <v>0</v>
-      </c>
+      <c r="B128" s="15"/>
       <c r="C128" s="2"/>
       <c r="D128" s="16"/>
       <c r="E128" s="15"/>
@@ -3087,9 +2953,7 @@
     </row>
     <row r="129" spans="1:11">
       <c r="A129" s="1"/>
-      <c r="B129" s="15">
-        <v>0</v>
-      </c>
+      <c r="B129" s="15"/>
       <c r="C129" s="2"/>
       <c r="D129" s="16"/>
       <c r="E129" s="15"/>
@@ -3100,37 +2964,66 @@
       <c r="J129" s="15"/>
       <c r="K129" s="15"/>
     </row>
+    <row r="130" spans="1:11">
+      <c r="A130" s="1"/>
+      <c r="B130" s="15"/>
+      <c r="C130" s="2"/>
+      <c r="D130" s="16"/>
+      <c r="E130" s="15"/>
+      <c r="F130" s="15"/>
+      <c r="G130" s="15"/>
+      <c r="H130" s="15"/>
+      <c r="I130" s="15"/>
+      <c r="J130" s="15"/>
+      <c r="K130" s="15"/>
+    </row>
+    <row r="131" spans="1:11">
+      <c r="A131" s="1"/>
+      <c r="B131" s="15"/>
+      <c r="C131" s="2"/>
+      <c r="D131" s="16"/>
+      <c r="E131" s="15"/>
+      <c r="F131" s="15"/>
+      <c r="G131" s="15"/>
+      <c r="H131" s="15"/>
+      <c r="I131" s="15"/>
+      <c r="J131" s="15"/>
+      <c r="K131" s="15"/>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:C1"/>
+  </mergeCells>
   <phoneticPr fontId="5"/>
-  <dataValidations count="5">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B129">
+  <dataValidations disablePrompts="1" count="5">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:B131">
       <formula1>"0,1,2,3,4,5,6,7,8,9,10,11,12,13,14,15,16"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="0-127" prompt="If don't use CC set cell value empty" sqref="H2:I129">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="0-127" prompt="If don't use CC set cell value empty" sqref="H4:I131">
       <formula1>0</formula1>
       <formula2>127</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="0-127" prompt="If don't use MIDI Note on, set cell value empty." sqref="G2:G129">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="0-127" prompt="If don't use MIDI Note on, set cell value empty." sqref="G4:G131">
       <formula1>0</formula1>
       <formula2>127</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="0-127" prompt="If don't use Program Change, set cell value empty." sqref="J2:J129">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="0-127" prompt="If don't use Program Change, set cell value empty." sqref="J4:J131">
       <formula1>0</formula1>
       <formula2>127</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="0-127" prompt="If cell value is empty, MSB will be set 0._x000a__x000a_By my research, Maybe Cubase will not recognize MSB." sqref="K2:K129">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="0-127" prompt="If cell value is empty, MSB will be set 0._x000a__x000a_By my research, Maybe Cubase will not recognize MSB." sqref="K4:K131">
       <formula1>0</formula1>
       <formula2>127</formula2>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <drawing r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="3">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>'DO NOT MODIFY!'!$B$2:$B$4</xm:f>
@@ -3138,7 +3031,7 @@
           <x14:formula2>
             <xm:f>0</xm:f>
           </x14:formula2>
-          <xm:sqref>D2:D129</xm:sqref>
+          <xm:sqref>D4:D131</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
@@ -3147,7 +3040,7 @@
           <x14:formula2>
             <xm:f>0</xm:f>
           </x14:formula2>
-          <xm:sqref>E2:E129</xm:sqref>
+          <xm:sqref>E4:E131</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" promptTitle="MIDI Note" prompt="Choose from Drop-down list or imput number directly(0-127)_x000a__x000a_If don’t use MIDI Note, set Cell value empty.">
           <x14:formula1>
@@ -3156,7 +3049,7 @@
           <x14:formula2>
             <xm:f>0</xm:f>
           </x14:formula2>
-          <xm:sqref>F2:F129</xm:sqref>
+          <xm:sqref>F4:F131</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -3169,7 +3062,7 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <tabColor rgb="FF000000"/>
   </sheetPr>
-  <dimension ref="A1:C258"/>
+  <dimension ref="A1:E258"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3178,11 +3071,13 @@
     <col min="1" max="1" width="18.5" style="5" customWidth="1"/>
     <col min="2" max="2" width="20" style="5" customWidth="1"/>
     <col min="3" max="3" width="17.375" style="5" customWidth="1"/>
-    <col min="4" max="1025" width="9.875" style="5" customWidth="1"/>
+    <col min="4" max="4" width="18.875" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.625" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="1025" width="9.875" style="5" customWidth="1"/>
     <col min="1026" max="16384" width="8.875" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="23.25" customHeight="1">
+    <row r="1" spans="1:5" ht="23.25" customHeight="1">
       <c r="A1" s="3" t="s">
         <v>15</v>
       </c>
@@ -3192,13 +3087,21 @@
       <c r="C1" s="4" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
+      <c r="D1" s="25" t="s">
+        <v>144</v>
+      </c>
+      <c r="E1" s="25" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2" s="6"/>
       <c r="B2" s="7"/>
       <c r="C2" s="6"/>
-    </row>
-    <row r="3" spans="1:3">
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3" s="1" t="s">
         <v>14</v>
       </c>
@@ -3208,8 +3111,14 @@
       <c r="C3" s="6">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:3">
+      <c r="D3" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="24" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4" s="1" t="s">
         <v>16</v>
       </c>
@@ -3219,8 +3128,14 @@
       <c r="C4" s="6">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:3">
+      <c r="D4" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" s="24" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5" s="1" t="s">
         <v>18</v>
       </c>
@@ -3228,8 +3143,14 @@
       <c r="C5" s="6">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:3">
+      <c r="D5" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" s="24" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
       <c r="A6" s="1" t="s">
         <v>19</v>
       </c>
@@ -3237,899 +3158,1661 @@
       <c r="C6" s="6">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:3">
+      <c r="D6" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" s="24" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
       <c r="A7" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B7" s="8"/>
-    </row>
-    <row r="8" spans="1:3">
+      <c r="D7" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7" s="24" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
       <c r="A8" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B8" s="8"/>
-    </row>
-    <row r="9" spans="1:3">
+      <c r="D8" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="E8" s="24" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
       <c r="A9" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B9" s="8"/>
-    </row>
-    <row r="10" spans="1:3">
+      <c r="D9" s="24" t="s">
+        <v>27</v>
+      </c>
+      <c r="E9" s="24" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
       <c r="A10" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B10" s="8"/>
-    </row>
-    <row r="11" spans="1:3">
+      <c r="D10" s="24" t="s">
+        <v>28</v>
+      </c>
+      <c r="E10" s="24" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
       <c r="A11" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B11" s="8"/>
-    </row>
-    <row r="12" spans="1:3">
+      <c r="D11" s="24" t="s">
+        <v>30</v>
+      </c>
+      <c r="E11" s="24" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
       <c r="A12" s="1" t="s">
         <v>25</v>
       </c>
       <c r="B12" s="8"/>
-    </row>
-    <row r="13" spans="1:3">
+      <c r="D12" s="24" t="s">
+        <v>32</v>
+      </c>
+      <c r="E12" s="24" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
       <c r="A13" s="1" t="s">
         <v>26</v>
       </c>
       <c r="B13" s="8"/>
-    </row>
-    <row r="14" spans="1:3">
+      <c r="D13" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="E13" s="24" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
       <c r="A14" s="1" t="s">
         <v>27</v>
       </c>
       <c r="B14" s="8"/>
-    </row>
-    <row r="15" spans="1:3">
+      <c r="D14" s="24" t="s">
+        <v>35</v>
+      </c>
+      <c r="E14" s="24" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
       <c r="A15" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B15" s="8"/>
-    </row>
-    <row r="16" spans="1:3">
+      <c r="D15" s="24" t="s">
+        <v>37</v>
+      </c>
+      <c r="E15" s="24" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
       <c r="A16" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B16" s="8"/>
-    </row>
-    <row r="17" spans="1:2">
+      <c r="D16" s="24" t="s">
+        <v>39</v>
+      </c>
+      <c r="E16" s="24" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
       <c r="A17" s="1" t="s">
         <v>30</v>
       </c>
       <c r="B17" s="8"/>
-    </row>
-    <row r="18" spans="1:2">
+      <c r="D17" s="24" t="s">
+        <v>40</v>
+      </c>
+      <c r="E17" s="24" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
       <c r="A18" s="1" t="s">
         <v>31</v>
       </c>
       <c r="B18" s="8"/>
-    </row>
-    <row r="19" spans="1:2">
+      <c r="D18" s="24" t="s">
+        <v>42</v>
+      </c>
+      <c r="E18" s="24" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
       <c r="A19" s="1" t="s">
         <v>32</v>
       </c>
       <c r="B19" s="8"/>
-    </row>
-    <row r="20" spans="1:2">
+      <c r="D19" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="E19" s="24" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
       <c r="A20" s="1" t="s">
         <v>33</v>
       </c>
       <c r="B20" s="8"/>
-    </row>
-    <row r="21" spans="1:2">
+      <c r="D20" s="24" t="s">
+        <v>45</v>
+      </c>
+      <c r="E20" s="24" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
       <c r="A21" s="1" t="s">
         <v>34</v>
       </c>
       <c r="B21" s="8"/>
-    </row>
-    <row r="22" spans="1:2">
+      <c r="D21" s="24" t="s">
+        <v>47</v>
+      </c>
+      <c r="E21" s="24" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
       <c r="A22" s="1" t="s">
         <v>35</v>
       </c>
       <c r="B22" s="8"/>
-    </row>
-    <row r="23" spans="1:2">
+      <c r="D22" s="24" t="s">
+        <v>49</v>
+      </c>
+      <c r="E22" s="24" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
       <c r="A23" s="1" t="s">
         <v>36</v>
       </c>
       <c r="B23" s="8"/>
-    </row>
-    <row r="24" spans="1:2">
+      <c r="D23" s="24" t="s">
+        <v>51</v>
+      </c>
+      <c r="E23" s="24" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
       <c r="A24" s="1" t="s">
         <v>37</v>
       </c>
       <c r="B24" s="8"/>
-    </row>
-    <row r="25" spans="1:2">
+      <c r="D24" s="24" t="s">
+        <v>52</v>
+      </c>
+      <c r="E24" s="24" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
       <c r="A25" s="1" t="s">
         <v>38</v>
       </c>
       <c r="B25" s="8"/>
-    </row>
-    <row r="26" spans="1:2">
+      <c r="D25" s="24" t="s">
+        <v>54</v>
+      </c>
+      <c r="E25" s="24" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
       <c r="A26" s="1" t="s">
         <v>39</v>
       </c>
       <c r="B26" s="8"/>
-    </row>
-    <row r="27" spans="1:2">
+      <c r="D26" s="24" t="s">
+        <v>56</v>
+      </c>
+      <c r="E26" s="24" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
       <c r="A27" s="1" t="s">
         <v>40</v>
       </c>
       <c r="B27" s="8"/>
-    </row>
-    <row r="28" spans="1:2">
+      <c r="D27" s="24" t="s">
+        <v>57</v>
+      </c>
+      <c r="E27" s="24" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
       <c r="A28" s="1" t="s">
         <v>41</v>
       </c>
       <c r="B28" s="8"/>
-    </row>
-    <row r="29" spans="1:2">
+      <c r="D28" s="24" t="s">
+        <v>59</v>
+      </c>
+      <c r="E28" s="24" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
       <c r="A29" s="1" t="s">
         <v>42</v>
       </c>
       <c r="B29" s="8"/>
-    </row>
-    <row r="30" spans="1:2">
+      <c r="D29" s="24" t="s">
+        <v>61</v>
+      </c>
+      <c r="E29" s="24" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
       <c r="A30" s="1" t="s">
         <v>43</v>
       </c>
       <c r="B30" s="8"/>
-    </row>
-    <row r="31" spans="1:2">
+      <c r="D30" s="24" t="s">
+        <v>63</v>
+      </c>
+      <c r="E30" s="24" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
       <c r="A31" s="1" t="s">
         <v>44</v>
       </c>
       <c r="B31" s="8"/>
-    </row>
-    <row r="32" spans="1:2">
+      <c r="D31" s="24" t="s">
+        <v>64</v>
+      </c>
+      <c r="E31" s="24" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
       <c r="A32" s="1" t="s">
         <v>45</v>
       </c>
       <c r="B32" s="8"/>
-    </row>
-    <row r="33" spans="1:2">
+      <c r="D32" s="24" t="s">
+        <v>66</v>
+      </c>
+      <c r="E32" s="24" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
       <c r="A33" s="1" t="s">
         <v>46</v>
       </c>
       <c r="B33" s="8"/>
-    </row>
-    <row r="34" spans="1:2">
+      <c r="D33" s="24" t="s">
+        <v>68</v>
+      </c>
+      <c r="E33" s="24" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
       <c r="A34" s="1" t="s">
         <v>47</v>
       </c>
       <c r="B34" s="8"/>
-    </row>
-    <row r="35" spans="1:2">
+      <c r="D34" s="24" t="s">
+        <v>69</v>
+      </c>
+      <c r="E34" s="24" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
       <c r="A35" s="1" t="s">
         <v>48</v>
       </c>
       <c r="B35" s="8"/>
-    </row>
-    <row r="36" spans="1:2">
+      <c r="D35" s="24" t="s">
+        <v>71</v>
+      </c>
+      <c r="E35" s="24" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
       <c r="A36" s="1" t="s">
         <v>49</v>
       </c>
       <c r="B36" s="8"/>
-    </row>
-    <row r="37" spans="1:2">
+      <c r="D36" s="24" t="s">
+        <v>73</v>
+      </c>
+      <c r="E36" s="24" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
       <c r="A37" s="1" t="s">
         <v>50</v>
       </c>
       <c r="B37" s="8"/>
-    </row>
-    <row r="38" spans="1:2">
+      <c r="D37" s="24" t="s">
+        <v>75</v>
+      </c>
+      <c r="E37" s="24" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5">
       <c r="A38" s="1" t="s">
         <v>51</v>
       </c>
       <c r="B38" s="8"/>
-    </row>
-    <row r="39" spans="1:2">
+      <c r="D38" s="24" t="s">
+        <v>76</v>
+      </c>
+      <c r="E38" s="24" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5">
       <c r="A39" s="1" t="s">
         <v>52</v>
       </c>
       <c r="B39" s="8"/>
-    </row>
-    <row r="40" spans="1:2">
+      <c r="D39" s="24" t="s">
+        <v>78</v>
+      </c>
+      <c r="E39" s="24" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5">
       <c r="A40" s="1" t="s">
         <v>53</v>
       </c>
       <c r="B40" s="8"/>
-    </row>
-    <row r="41" spans="1:2">
+      <c r="D40" s="24" t="s">
+        <v>80</v>
+      </c>
+      <c r="E40" s="24" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5">
       <c r="A41" s="1" t="s">
         <v>54</v>
       </c>
       <c r="B41" s="8"/>
-    </row>
-    <row r="42" spans="1:2">
+      <c r="D41" s="24" t="s">
+        <v>81</v>
+      </c>
+      <c r="E41" s="24" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5">
       <c r="A42" s="1" t="s">
         <v>55</v>
       </c>
       <c r="B42" s="8"/>
-    </row>
-    <row r="43" spans="1:2">
+      <c r="D42" s="24" t="s">
+        <v>83</v>
+      </c>
+      <c r="E42" s="24" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5">
       <c r="A43" s="1" t="s">
         <v>56</v>
       </c>
       <c r="B43" s="8"/>
-    </row>
-    <row r="44" spans="1:2">
+      <c r="D43" s="24" t="s">
+        <v>85</v>
+      </c>
+      <c r="E43" s="24" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5">
       <c r="A44" s="1" t="s">
         <v>57</v>
       </c>
       <c r="B44" s="8"/>
-    </row>
-    <row r="45" spans="1:2">
+      <c r="D44" s="24" t="s">
+        <v>87</v>
+      </c>
+      <c r="E44" s="24" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5">
       <c r="A45" s="1" t="s">
         <v>58</v>
       </c>
       <c r="B45" s="8"/>
-    </row>
-    <row r="46" spans="1:2">
+      <c r="D45" s="24" t="s">
+        <v>88</v>
+      </c>
+      <c r="E45" s="24" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5">
       <c r="A46" s="1" t="s">
         <v>59</v>
       </c>
       <c r="B46" s="8"/>
-    </row>
-    <row r="47" spans="1:2">
+      <c r="D46" s="24" t="s">
+        <v>90</v>
+      </c>
+      <c r="E46" s="24" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5">
       <c r="A47" s="1" t="s">
         <v>60</v>
       </c>
       <c r="B47" s="8"/>
-    </row>
-    <row r="48" spans="1:2">
+      <c r="D47" s="24" t="s">
+        <v>92</v>
+      </c>
+      <c r="E47" s="24" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5">
       <c r="A48" s="1" t="s">
         <v>61</v>
       </c>
       <c r="B48" s="8"/>
-    </row>
-    <row r="49" spans="1:2">
+      <c r="D48" s="24" t="s">
+        <v>93</v>
+      </c>
+      <c r="E48" s="24" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5">
       <c r="A49" s="1" t="s">
         <v>62</v>
       </c>
       <c r="B49" s="8"/>
-    </row>
-    <row r="50" spans="1:2">
+      <c r="D49" s="24" t="s">
+        <v>95</v>
+      </c>
+      <c r="E49" s="24" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5">
       <c r="A50" s="1" t="s">
         <v>63</v>
       </c>
       <c r="B50" s="8"/>
-    </row>
-    <row r="51" spans="1:2">
+      <c r="D50" s="24" t="s">
+        <v>97</v>
+      </c>
+      <c r="E50" s="24" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5">
       <c r="A51" s="1" t="s">
         <v>64</v>
       </c>
       <c r="B51" s="8"/>
-    </row>
-    <row r="52" spans="1:2">
+      <c r="D51" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="E51" s="24" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5">
       <c r="A52" s="1" t="s">
         <v>65</v>
       </c>
       <c r="B52" s="8"/>
-    </row>
-    <row r="53" spans="1:2">
+      <c r="D52" s="24" t="s">
+        <v>100</v>
+      </c>
+      <c r="E52" s="24" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5">
       <c r="A53" s="1" t="s">
         <v>66</v>
       </c>
       <c r="B53" s="8"/>
-    </row>
-    <row r="54" spans="1:2">
+      <c r="D53" s="24" t="s">
+        <v>102</v>
+      </c>
+      <c r="E53" s="24" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5">
       <c r="A54" s="1" t="s">
         <v>67</v>
       </c>
       <c r="B54" s="8"/>
-    </row>
-    <row r="55" spans="1:2">
+      <c r="D54" s="24" t="s">
+        <v>104</v>
+      </c>
+      <c r="E54" s="24" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5">
       <c r="A55" s="1" t="s">
         <v>68</v>
       </c>
       <c r="B55" s="8"/>
-    </row>
-    <row r="56" spans="1:2">
+      <c r="D55" s="24" t="s">
+        <v>105</v>
+      </c>
+      <c r="E55" s="24" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5">
       <c r="A56" s="1" t="s">
         <v>69</v>
       </c>
       <c r="B56" s="8"/>
-    </row>
-    <row r="57" spans="1:2">
+      <c r="D56" s="24" t="s">
+        <v>107</v>
+      </c>
+      <c r="E56" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5">
       <c r="A57" s="1" t="s">
         <v>70</v>
       </c>
       <c r="B57" s="8"/>
-    </row>
-    <row r="58" spans="1:2">
+      <c r="D57" s="24" t="s">
+        <v>109</v>
+      </c>
+      <c r="E57" s="24">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5">
       <c r="A58" s="1" t="s">
         <v>71</v>
       </c>
       <c r="B58" s="8"/>
-    </row>
-    <row r="59" spans="1:2">
+      <c r="D58" s="24" t="s">
+        <v>111</v>
+      </c>
+      <c r="E58" s="24">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5">
       <c r="A59" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B59" s="8"/>
-    </row>
-    <row r="60" spans="1:2">
+      <c r="D59" s="24" t="s">
+        <v>112</v>
+      </c>
+      <c r="E59" s="24">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5">
       <c r="A60" s="1" t="s">
         <v>73</v>
       </c>
       <c r="B60" s="8"/>
-    </row>
-    <row r="61" spans="1:2">
+      <c r="D60" s="24" t="s">
+        <v>114</v>
+      </c>
+      <c r="E60" s="24">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5">
       <c r="A61" s="1" t="s">
         <v>74</v>
       </c>
       <c r="B61" s="8"/>
-    </row>
-    <row r="62" spans="1:2">
+      <c r="D61" s="24" t="s">
+        <v>116</v>
+      </c>
+      <c r="E61" s="24">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5">
       <c r="A62" s="1" t="s">
         <v>75</v>
       </c>
       <c r="B62" s="8"/>
-    </row>
-    <row r="63" spans="1:2">
+      <c r="D62" s="24" t="s">
+        <v>117</v>
+      </c>
+      <c r="E62" s="24">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5">
       <c r="A63" s="1" t="s">
         <v>76</v>
       </c>
       <c r="B63" s="8"/>
-    </row>
-    <row r="64" spans="1:2">
+      <c r="D63" s="24" t="s">
+        <v>119</v>
+      </c>
+      <c r="E63" s="24">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5">
       <c r="A64" s="1" t="s">
         <v>77</v>
       </c>
       <c r="B64" s="8"/>
-    </row>
-    <row r="65" spans="1:2">
+      <c r="D64" s="24" t="s">
+        <v>121</v>
+      </c>
+      <c r="E64" s="24">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5">
       <c r="A65" s="1" t="s">
         <v>78</v>
       </c>
       <c r="B65" s="8"/>
-    </row>
-    <row r="66" spans="1:2">
+      <c r="D65" s="24" t="s">
+        <v>123</v>
+      </c>
+      <c r="E65" s="24">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5">
       <c r="A66" s="1" t="s">
         <v>79</v>
       </c>
       <c r="B66" s="8"/>
-    </row>
-    <row r="67" spans="1:2">
+      <c r="D66" s="24" t="s">
+        <v>124</v>
+      </c>
+      <c r="E66" s="24">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5">
       <c r="A67" s="1" t="s">
         <v>80</v>
       </c>
       <c r="B67" s="8"/>
-    </row>
-    <row r="68" spans="1:2">
+      <c r="D67" s="24" t="s">
+        <v>126</v>
+      </c>
+      <c r="E67" s="24">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5">
       <c r="A68" s="1" t="s">
         <v>81</v>
       </c>
       <c r="B68" s="8"/>
-    </row>
-    <row r="69" spans="1:2">
+      <c r="D68" s="24" t="s">
+        <v>128</v>
+      </c>
+      <c r="E68" s="24">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5">
       <c r="A69" s="1" t="s">
         <v>82</v>
       </c>
       <c r="B69" s="8"/>
-    </row>
-    <row r="70" spans="1:2">
+      <c r="D69" s="24" t="s">
+        <v>129</v>
+      </c>
+      <c r="E69" s="24">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5">
       <c r="A70" s="1" t="s">
         <v>83</v>
       </c>
       <c r="B70" s="8"/>
-    </row>
-    <row r="71" spans="1:2">
+      <c r="D70" s="24" t="s">
+        <v>131</v>
+      </c>
+      <c r="E70" s="24">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5">
       <c r="A71" s="1" t="s">
         <v>84</v>
       </c>
       <c r="B71" s="8"/>
-    </row>
-    <row r="72" spans="1:2">
+      <c r="D71" s="24" t="s">
+        <v>133</v>
+      </c>
+      <c r="E71" s="24">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5">
       <c r="A72" s="1" t="s">
         <v>85</v>
       </c>
       <c r="B72" s="8"/>
-    </row>
-    <row r="73" spans="1:2">
+      <c r="D72" s="24" t="s">
+        <v>135</v>
+      </c>
+      <c r="E72" s="24">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5">
       <c r="A73" s="1" t="s">
         <v>86</v>
       </c>
       <c r="B73" s="8"/>
-    </row>
-    <row r="74" spans="1:2">
+      <c r="D73" s="24" t="s">
+        <v>136</v>
+      </c>
+      <c r="E73" s="24">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5">
       <c r="A74" s="1" t="s">
         <v>87</v>
       </c>
       <c r="B74" s="8"/>
-    </row>
-    <row r="75" spans="1:2">
+      <c r="D74" s="24" t="s">
+        <v>138</v>
+      </c>
+      <c r="E74" s="24">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5">
       <c r="A75" s="1" t="s">
         <v>88</v>
       </c>
       <c r="B75" s="8"/>
-    </row>
-    <row r="76" spans="1:2">
+      <c r="D75" s="24" t="s">
+        <v>140</v>
+      </c>
+      <c r="E75" s="24">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5">
       <c r="A76" s="1" t="s">
         <v>89</v>
       </c>
       <c r="B76" s="8"/>
-    </row>
-    <row r="77" spans="1:2">
+      <c r="D76" s="24" t="s">
+        <v>141</v>
+      </c>
+      <c r="E76" s="24">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5">
       <c r="A77" s="1" t="s">
         <v>90</v>
       </c>
       <c r="B77" s="8"/>
-    </row>
-    <row r="78" spans="1:2">
+      <c r="D77" s="24" t="s">
+        <v>143</v>
+      </c>
+      <c r="E77" s="24">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5">
       <c r="A78" s="1" t="s">
         <v>91</v>
       </c>
       <c r="B78" s="8"/>
-    </row>
-    <row r="79" spans="1:2">
+      <c r="D78" s="24">
+        <v>0</v>
+      </c>
+      <c r="E78" s="24">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5">
       <c r="A79" s="1" t="s">
         <v>92</v>
       </c>
       <c r="B79" s="8"/>
-    </row>
-    <row r="80" spans="1:2">
+      <c r="D79" s="24">
+        <v>2</v>
+      </c>
+      <c r="E79" s="24">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5">
       <c r="A80" s="1" t="s">
         <v>93</v>
       </c>
       <c r="B80" s="8"/>
-    </row>
-    <row r="81" spans="1:2">
+      <c r="D80" s="24">
+        <v>4</v>
+      </c>
+      <c r="E80" s="24">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5">
       <c r="A81" s="1" t="s">
         <v>94</v>
       </c>
       <c r="B81" s="8"/>
-    </row>
-    <row r="82" spans="1:2">
+      <c r="D81" s="24">
+        <v>5</v>
+      </c>
+      <c r="E81" s="24">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5">
       <c r="A82" s="1" t="s">
         <v>95</v>
       </c>
       <c r="B82" s="8"/>
-    </row>
-    <row r="83" spans="1:2">
+      <c r="D82" s="24">
+        <v>7</v>
+      </c>
+      <c r="E82" s="24">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5">
       <c r="A83" s="1" t="s">
         <v>96</v>
       </c>
       <c r="B83" s="8"/>
-    </row>
-    <row r="84" spans="1:2">
+      <c r="D83" s="24">
+        <v>9</v>
+      </c>
+      <c r="E83" s="24">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5">
       <c r="A84" s="1" t="s">
         <v>97</v>
       </c>
       <c r="B84" s="8"/>
-    </row>
-    <row r="85" spans="1:2">
+      <c r="D84" s="24">
+        <v>11</v>
+      </c>
+      <c r="E84" s="24">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5">
       <c r="A85" s="1" t="s">
         <v>98</v>
       </c>
       <c r="B85" s="8"/>
-    </row>
-    <row r="86" spans="1:2">
+      <c r="D85" s="24">
+        <v>12</v>
+      </c>
+      <c r="E85" s="24">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5">
       <c r="A86" s="1" t="s">
         <v>99</v>
       </c>
       <c r="B86" s="8"/>
-    </row>
-    <row r="87" spans="1:2">
+      <c r="D86" s="24">
+        <v>14</v>
+      </c>
+      <c r="E86" s="24">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5">
       <c r="A87" s="1" t="s">
         <v>100</v>
       </c>
       <c r="B87" s="8"/>
-    </row>
-    <row r="88" spans="1:2">
+      <c r="D87" s="24">
+        <v>16</v>
+      </c>
+      <c r="E87" s="24">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5">
       <c r="A88" s="1" t="s">
         <v>101</v>
       </c>
       <c r="B88" s="8"/>
-    </row>
-    <row r="89" spans="1:2">
+      <c r="D88" s="24">
+        <v>17</v>
+      </c>
+      <c r="E88" s="24">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5">
       <c r="A89" s="1" t="s">
         <v>102</v>
       </c>
       <c r="B89" s="8"/>
-    </row>
-    <row r="90" spans="1:2">
+      <c r="D89" s="24">
+        <v>19</v>
+      </c>
+      <c r="E89" s="24">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5">
       <c r="A90" s="1" t="s">
         <v>103</v>
       </c>
       <c r="B90" s="8"/>
-    </row>
-    <row r="91" spans="1:2">
+      <c r="D90" s="24">
+        <v>21</v>
+      </c>
+      <c r="E90" s="24">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5">
       <c r="A91" s="1" t="s">
         <v>104</v>
       </c>
       <c r="B91" s="8"/>
-    </row>
-    <row r="92" spans="1:2">
+      <c r="D91" s="24">
+        <v>23</v>
+      </c>
+      <c r="E91" s="24">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5">
       <c r="A92" s="1" t="s">
         <v>105</v>
       </c>
       <c r="B92" s="8"/>
-    </row>
-    <row r="93" spans="1:2">
+      <c r="D92" s="24">
+        <v>24</v>
+      </c>
+      <c r="E92" s="24">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5">
       <c r="A93" s="1" t="s">
         <v>106</v>
       </c>
       <c r="B93" s="8"/>
-    </row>
-    <row r="94" spans="1:2">
+      <c r="D93" s="24">
+        <v>26</v>
+      </c>
+      <c r="E93" s="24">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5">
       <c r="A94" s="1" t="s">
         <v>107</v>
       </c>
       <c r="B94" s="8"/>
-    </row>
-    <row r="95" spans="1:2">
+      <c r="D94" s="24">
+        <v>28</v>
+      </c>
+      <c r="E94" s="24">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5">
       <c r="A95" s="1" t="s">
         <v>108</v>
       </c>
       <c r="B95" s="8"/>
-    </row>
-    <row r="96" spans="1:2">
+      <c r="D95" s="24">
+        <v>29</v>
+      </c>
+      <c r="E95" s="24">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5">
       <c r="A96" s="1" t="s">
         <v>109</v>
       </c>
       <c r="B96" s="8"/>
-    </row>
-    <row r="97" spans="1:2">
+      <c r="D96" s="24">
+        <v>31</v>
+      </c>
+      <c r="E96" s="24">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5">
       <c r="A97" s="1" t="s">
         <v>110</v>
       </c>
       <c r="B97" s="8"/>
-    </row>
-    <row r="98" spans="1:2">
+      <c r="D97" s="24">
+        <v>33</v>
+      </c>
+      <c r="E97" s="24">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5">
       <c r="A98" s="1" t="s">
         <v>111</v>
       </c>
       <c r="B98" s="8"/>
-    </row>
-    <row r="99" spans="1:2">
+      <c r="D98" s="24">
+        <v>35</v>
+      </c>
+      <c r="E98" s="24">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5">
       <c r="A99" s="1" t="s">
         <v>112</v>
       </c>
       <c r="B99" s="8"/>
-    </row>
-    <row r="100" spans="1:2">
+      <c r="D99" s="24">
+        <v>36</v>
+      </c>
+      <c r="E99" s="24">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5">
       <c r="A100" s="1" t="s">
         <v>113</v>
       </c>
       <c r="B100" s="8"/>
-    </row>
-    <row r="101" spans="1:2">
+      <c r="D100" s="24">
+        <v>38</v>
+      </c>
+      <c r="E100" s="24">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5">
       <c r="A101" s="1" t="s">
         <v>114</v>
       </c>
       <c r="B101" s="8"/>
-    </row>
-    <row r="102" spans="1:2">
+      <c r="D101" s="24">
+        <v>40</v>
+      </c>
+      <c r="E101" s="24">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5">
       <c r="A102" s="1" t="s">
         <v>115</v>
       </c>
       <c r="B102" s="8"/>
-    </row>
-    <row r="103" spans="1:2">
+      <c r="D102" s="24">
+        <v>41</v>
+      </c>
+      <c r="E102" s="24">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5">
       <c r="A103" s="1" t="s">
         <v>116</v>
       </c>
       <c r="B103" s="8"/>
-    </row>
-    <row r="104" spans="1:2">
+      <c r="D103" s="24">
+        <v>43</v>
+      </c>
+      <c r="E103" s="24">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5">
       <c r="A104" s="1" t="s">
         <v>117</v>
       </c>
       <c r="B104" s="8"/>
-    </row>
-    <row r="105" spans="1:2">
+      <c r="D104" s="24">
+        <v>45</v>
+      </c>
+      <c r="E104" s="24">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5">
       <c r="A105" s="1" t="s">
         <v>118</v>
       </c>
       <c r="B105" s="8"/>
-    </row>
-    <row r="106" spans="1:2">
+      <c r="D105" s="24">
+        <v>47</v>
+      </c>
+      <c r="E105" s="24">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5">
       <c r="A106" s="1" t="s">
         <v>119</v>
       </c>
       <c r="B106" s="8"/>
-    </row>
-    <row r="107" spans="1:2">
+      <c r="D106" s="24">
+        <v>48</v>
+      </c>
+      <c r="E106" s="24">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5">
       <c r="A107" s="1" t="s">
         <v>120</v>
       </c>
       <c r="B107" s="8"/>
-    </row>
-    <row r="108" spans="1:2">
+      <c r="D107" s="24">
+        <v>50</v>
+      </c>
+      <c r="E107" s="24">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5">
       <c r="A108" s="1" t="s">
         <v>121</v>
       </c>
       <c r="B108" s="8"/>
-    </row>
-    <row r="109" spans="1:2">
+      <c r="D108" s="24">
+        <v>52</v>
+      </c>
+      <c r="E108" s="24">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5">
       <c r="A109" s="1" t="s">
         <v>122</v>
       </c>
       <c r="B109" s="8"/>
-    </row>
-    <row r="110" spans="1:2">
+      <c r="D109" s="24">
+        <v>53</v>
+      </c>
+      <c r="E109" s="23"/>
+    </row>
+    <row r="110" spans="1:5">
       <c r="A110" s="1" t="s">
         <v>123</v>
       </c>
       <c r="B110" s="8"/>
-    </row>
-    <row r="111" spans="1:2">
+      <c r="D110" s="24">
+        <v>55</v>
+      </c>
+      <c r="E110" s="23"/>
+    </row>
+    <row r="111" spans="1:5">
       <c r="A111" s="1" t="s">
         <v>124</v>
       </c>
       <c r="B111" s="8"/>
-    </row>
-    <row r="112" spans="1:2">
+      <c r="D111" s="24">
+        <v>57</v>
+      </c>
+      <c r="E111" s="23"/>
+    </row>
+    <row r="112" spans="1:5">
       <c r="A112" s="1" t="s">
         <v>125</v>
       </c>
       <c r="B112" s="8"/>
-    </row>
-    <row r="113" spans="1:2">
+      <c r="D112" s="24">
+        <v>59</v>
+      </c>
+      <c r="E112" s="23"/>
+    </row>
+    <row r="113" spans="1:4">
       <c r="A113" s="1" t="s">
         <v>126</v>
       </c>
       <c r="B113" s="8"/>
-    </row>
-    <row r="114" spans="1:2">
+      <c r="D113" s="24">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4">
       <c r="A114" s="1" t="s">
         <v>127</v>
       </c>
       <c r="B114" s="8"/>
-    </row>
-    <row r="115" spans="1:2">
+      <c r="D114" s="24">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4">
       <c r="A115" s="1" t="s">
         <v>128</v>
       </c>
       <c r="B115" s="8"/>
-    </row>
-    <row r="116" spans="1:2">
+      <c r="D115" s="24">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4">
       <c r="A116" s="1" t="s">
         <v>129</v>
       </c>
       <c r="B116" s="8"/>
-    </row>
-    <row r="117" spans="1:2">
+      <c r="D116" s="24">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4">
       <c r="A117" s="1" t="s">
         <v>130</v>
       </c>
       <c r="B117" s="8"/>
-    </row>
-    <row r="118" spans="1:2">
+      <c r="D117" s="24">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4">
       <c r="A118" s="1" t="s">
         <v>131</v>
       </c>
       <c r="B118" s="8"/>
-    </row>
-    <row r="119" spans="1:2">
+      <c r="D118" s="24">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4">
       <c r="A119" s="1" t="s">
         <v>132</v>
       </c>
       <c r="B119" s="8"/>
-    </row>
-    <row r="120" spans="1:2">
+      <c r="D119" s="24">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4">
       <c r="A120" s="1" t="s">
         <v>133</v>
       </c>
       <c r="B120" s="8"/>
-    </row>
-    <row r="121" spans="1:2">
+      <c r="D120" s="24">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4">
       <c r="A121" s="1" t="s">
         <v>134</v>
       </c>
       <c r="B121" s="8"/>
-    </row>
-    <row r="122" spans="1:2">
+      <c r="D121" s="24">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4">
       <c r="A122" s="1" t="s">
         <v>135</v>
       </c>
       <c r="B122" s="8"/>
-    </row>
-    <row r="123" spans="1:2">
+      <c r="D122" s="24">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4">
       <c r="A123" s="1" t="s">
         <v>136</v>
       </c>
       <c r="B123" s="8"/>
-    </row>
-    <row r="124" spans="1:2">
+      <c r="D123" s="24">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4">
       <c r="A124" s="1" t="s">
         <v>137</v>
       </c>
       <c r="B124" s="8"/>
-    </row>
-    <row r="125" spans="1:2">
+      <c r="D124" s="24">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4">
       <c r="A125" s="1" t="s">
         <v>138</v>
       </c>
       <c r="B125" s="8"/>
-    </row>
-    <row r="126" spans="1:2">
+      <c r="D125" s="24">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4">
       <c r="A126" s="1" t="s">
         <v>139</v>
       </c>
       <c r="B126" s="8"/>
-    </row>
-    <row r="127" spans="1:2">
+      <c r="D126" s="24">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4">
       <c r="A127" s="1" t="s">
         <v>140</v>
       </c>
       <c r="B127" s="8"/>
-    </row>
-    <row r="128" spans="1:2">
+      <c r="D127" s="24">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4">
       <c r="A128" s="1" t="s">
         <v>141</v>
       </c>
       <c r="B128" s="8"/>
-    </row>
-    <row r="129" spans="1:2">
+      <c r="D128" s="24">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4">
       <c r="A129" s="1" t="s">
         <v>142</v>
       </c>
       <c r="B129" s="8"/>
-    </row>
-    <row r="130" spans="1:2">
+      <c r="D129" s="24">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4">
       <c r="A130" s="1" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="131" spans="1:2">
+      <c r="D130" s="24">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4">
       <c r="A131" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="132" spans="1:2">
+      <c r="D131" s="24">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4">
       <c r="A132" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="133" spans="1:2">
+      <c r="D132" s="24">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4">
       <c r="A133" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="134" spans="1:2">
+      <c r="D133" s="24">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4">
       <c r="A134" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="135" spans="1:2">
+      <c r="D134" s="24">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4">
       <c r="A135" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="136" spans="1:2">
+      <c r="D135" s="24">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4">
       <c r="A136" s="1">
         <v>5</v>
       </c>
-    </row>
-    <row r="137" spans="1:2">
+      <c r="D136" s="24">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4">
       <c r="A137" s="1">
         <v>6</v>
       </c>
-    </row>
-    <row r="138" spans="1:2">
+      <c r="D137" s="24">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4">
       <c r="A138" s="1">
         <v>7</v>
       </c>
-    </row>
-    <row r="139" spans="1:2">
+      <c r="D138" s="24">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4">
       <c r="A139" s="1">
         <v>8</v>
       </c>
-    </row>
-    <row r="140" spans="1:2">
+      <c r="D139" s="24">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4">
       <c r="A140" s="1">
         <v>9</v>
       </c>
-    </row>
-    <row r="141" spans="1:2">
+      <c r="D140" s="24">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4">
       <c r="A141" s="1">
         <v>10</v>
       </c>
-    </row>
-    <row r="142" spans="1:2">
+      <c r="D141" s="24">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4">
       <c r="A142" s="1">
         <v>11</v>
       </c>
-    </row>
-    <row r="143" spans="1:2">
+      <c r="D142" s="24">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4">
       <c r="A143" s="1">
         <v>12</v>
       </c>
-    </row>
-    <row r="144" spans="1:2">
+      <c r="D143" s="24">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4">
       <c r="A144" s="1">
         <v>13</v>
       </c>
-    </row>
-    <row r="145" spans="1:1">
+      <c r="D144" s="24">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4">
       <c r="A145" s="1">
         <v>14</v>
       </c>
-    </row>
-    <row r="146" spans="1:1">
+      <c r="D145" s="24">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4">
       <c r="A146" s="1">
         <v>15</v>
       </c>
-    </row>
-    <row r="147" spans="1:1">
+      <c r="D146" s="24">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4">
       <c r="A147" s="1">
         <v>16</v>
       </c>
-    </row>
-    <row r="148" spans="1:1">
+      <c r="D147" s="24">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4">
       <c r="A148" s="1">
         <v>17</v>
       </c>
-    </row>
-    <row r="149" spans="1:1">
+      <c r="D148" s="24">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4">
       <c r="A149" s="1">
         <v>18</v>
       </c>
-    </row>
-    <row r="150" spans="1:1">
+      <c r="D149" s="24">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4">
       <c r="A150" s="1">
         <v>19</v>
       </c>
-    </row>
-    <row r="151" spans="1:1">
+      <c r="D150" s="24">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4">
       <c r="A151" s="1">
         <v>20</v>
       </c>
-    </row>
-    <row r="152" spans="1:1">
+      <c r="D151" s="24">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="152" spans="1:4">
       <c r="A152" s="1">
         <v>21</v>
       </c>
-    </row>
-    <row r="153" spans="1:1">
+      <c r="D152" s="24">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="153" spans="1:4">
       <c r="A153" s="1">
         <v>22</v>
       </c>
-    </row>
-    <row r="154" spans="1:1">
+      <c r="D153" s="23"/>
+    </row>
+    <row r="154" spans="1:4">
       <c r="A154" s="1">
         <v>23</v>
       </c>
-    </row>
-    <row r="155" spans="1:1">
+      <c r="D154" s="23"/>
+    </row>
+    <row r="155" spans="1:4">
       <c r="A155" s="1">
         <v>24</v>
       </c>
-    </row>
-    <row r="156" spans="1:1">
+      <c r="D155" s="23"/>
+    </row>
+    <row r="156" spans="1:4">
       <c r="A156" s="1">
         <v>25</v>
       </c>
-    </row>
-    <row r="157" spans="1:1">
+      <c r="D156" s="23"/>
+    </row>
+    <row r="157" spans="1:4">
       <c r="A157" s="1">
         <v>26</v>
       </c>
-    </row>
-    <row r="158" spans="1:1">
+      <c r="D157" s="23"/>
+    </row>
+    <row r="158" spans="1:4">
       <c r="A158" s="1">
         <v>27</v>
       </c>
-    </row>
-    <row r="159" spans="1:1">
+      <c r="D158" s="23"/>
+    </row>
+    <row r="159" spans="1:4">
       <c r="A159" s="1">
         <v>28</v>
       </c>
-    </row>
-    <row r="160" spans="1:1">
+      <c r="D159" s="23"/>
+    </row>
+    <row r="160" spans="1:4">
       <c r="A160" s="1">
         <v>29</v>
       </c>
+      <c r="D160" s="23"/>
     </row>
     <row r="161" spans="1:1">
       <c r="A161" s="1">

</xml_diff>